<commit_message>
updated class sheet (in forecast)
</commit_message>
<xml_diff>
--- a/cs_degree_planner/forecast/recommendcourses.xlsx
+++ b/cs_degree_planner/forecast/recommendcourses.xlsx
@@ -16,19 +16,19 @@
     <author/>
   </authors>
   <commentList>
-    <comment authorId="0" ref="C34">
+    <comment authorId="0" ref="C35">
       <text>
         <t xml:space="preserve">may never be offered
 	-ɱᴇᴇᴘᴇґ</t>
       </text>
     </comment>
-    <comment authorId="0" ref="C32">
+    <comment authorId="0" ref="C33">
       <text>
         <t xml:space="preserve">may never be offered
 	-ɱᴇᴇᴘᴇґ</t>
       </text>
     </comment>
-    <comment authorId="0" ref="C30">
+    <comment authorId="0" ref="C31">
       <text>
         <t xml:space="preserve">may never be offered
 	-ɱᴇᴇᴘᴇґ</t>
@@ -75,7 +75,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="521" uniqueCount="188">
   <si>
     <t>id</t>
   </si>
@@ -107,6 +107,12 @@
     <t>keywords</t>
   </si>
   <si>
+    <t>satisfyarea</t>
+  </si>
+  <si>
+    <t>notes</t>
+  </si>
+  <si>
     <t>CS</t>
   </si>
   <si>
@@ -116,6 +122,12 @@
     <t>Computer Science I</t>
   </si>
   <si>
+    <t>~</t>
+  </si>
+  <si>
+    <t>na</t>
+  </si>
+  <si>
     <t>WS</t>
   </si>
   <si>
@@ -128,7 +140,7 @@
     <t>Computer Science III</t>
   </si>
   <si>
-    <t>21200, 23210</t>
+    <t>212000, 232100</t>
   </si>
   <si>
     <t>Intermediate Data Structures</t>
@@ -146,42 +158,72 @@
     <t>Applied Cryptography</t>
   </si>
   <si>
+    <t>Cryptography, Cybersecurity</t>
+  </si>
+  <si>
+    <t>cselectiveunder</t>
+  </si>
+  <si>
     <t>Intro to Software Engineering</t>
   </si>
   <si>
+    <t>Software</t>
+  </si>
+  <si>
     <t>F</t>
   </si>
   <si>
     <t>User Interfaces</t>
   </si>
   <si>
-    <t>31400, 31300</t>
+    <t>UI</t>
+  </si>
+  <si>
+    <t>cselectiveover</t>
+  </si>
+  <si>
+    <t>314000, 313000</t>
   </si>
   <si>
     <t>Database Processing</t>
   </si>
   <si>
+    <t>Databases</t>
+  </si>
+  <si>
     <t>N</t>
   </si>
   <si>
     <t>Data Mining</t>
   </si>
   <si>
-    <t>31300, 31400</t>
+    <t>AI, Databases</t>
+  </si>
+  <si>
+    <t>313000, 314000</t>
   </si>
   <si>
     <t>Computational Science</t>
   </si>
   <si>
+    <t>Software, Databases</t>
+  </si>
+  <si>
     <t>S</t>
   </si>
   <si>
     <t>Game Programming</t>
   </si>
   <si>
+    <t>Games, Graphics, Teamwork</t>
+  </si>
+  <si>
     <t>Multi-agent Systems</t>
   </si>
   <si>
+    <t>AI</t>
+  </si>
+  <si>
     <t>C/C++ and Unix</t>
   </si>
   <si>
@@ -194,22 +236,37 @@
     <t>Intro Computer Graphics</t>
   </si>
   <si>
+    <t>Graphics</t>
+  </si>
+  <si>
     <t>Secure Software Development</t>
   </si>
   <si>
+    <t>Software, Cybersecurity</t>
+  </si>
+  <si>
     <t>Intro to Networks</t>
   </si>
   <si>
+    <t>Networks, Databases</t>
+  </si>
+  <si>
     <t>Intro to Parallel Computing</t>
   </si>
   <si>
-    <t>33000, 31300</t>
+    <t>HPC</t>
+  </si>
+  <si>
+    <t>330000, 313000</t>
   </si>
   <si>
     <t>Computer Architecture</t>
   </si>
   <si>
-    <t>33000, 31500</t>
+    <t>todo</t>
+  </si>
+  <si>
+    <t>330000, 315000</t>
   </si>
   <si>
     <t>Modeling and Simulation</t>
@@ -230,16 +287,25 @@
     <t>Advanced Data Structures</t>
   </si>
   <si>
+    <t>csmath, cselectiveover</t>
+  </si>
+  <si>
     <t>Automata Theory</t>
   </si>
   <si>
+    <t>does not exist?</t>
+  </si>
+  <si>
     <t>Probabilistic Methods for Artificial Intelligence</t>
   </si>
   <si>
     <t>Software Methology II</t>
   </si>
   <si>
-    <t>31400, 42500</t>
+    <t>Software, Teamwork</t>
+  </si>
+  <si>
+    <t>314000, 425000</t>
   </si>
   <si>
     <t>Introduction to Compilers</t>
@@ -248,7 +314,10 @@
     <t>Computer and Network Security</t>
   </si>
   <si>
-    <t>43300, 43200</t>
+    <t>Networks, Cybersecurity</t>
+  </si>
+  <si>
+    <t>433000, 432000</t>
   </si>
   <si>
     <t>Computer and Network Security II</t>
@@ -257,6 +326,9 @@
     <t>MATH</t>
   </si>
   <si>
+    <t>Elementary Functions</t>
+  </si>
+  <si>
     <t>Elements of Discrete Mathematics I</t>
   </si>
   <si>
@@ -266,12 +338,18 @@
     <t>Calculus I</t>
   </si>
   <si>
+    <t>default if don't like biology</t>
+  </si>
+  <si>
     <t>Calculus II</t>
   </si>
   <si>
     <t>Statistical Models/Methods</t>
   </si>
   <si>
+    <t>Statistics</t>
+  </si>
+  <si>
     <t>Elementary Linear Algebra I</t>
   </si>
   <si>
@@ -281,20 +359,293 @@
     <t>Calculus for the Biological Sciences I</t>
   </si>
   <si>
+    <t>Biology</t>
+  </si>
+  <si>
     <t>Calculus for the Biological Sciences II</t>
   </si>
   <si>
     <t>Calculus with Theory I</t>
   </si>
   <si>
+    <t>do not recommend</t>
+  </si>
+  <si>
     <t>Calculus with Theory II</t>
+  </si>
+  <si>
+    <t>PHYS</t>
+  </si>
+  <si>
+    <t>General Physics I</t>
+  </si>
+  <si>
+    <t>Physics</t>
+  </si>
+  <si>
+    <t>General Physics II</t>
+  </si>
+  <si>
+    <t>General Physics III</t>
+  </si>
+  <si>
+    <t>Foundations of Physics I</t>
+  </si>
+  <si>
+    <t>Physics, Advanced Physics</t>
+  </si>
+  <si>
+    <t>Foundations of Physics II</t>
+  </si>
+  <si>
+    <t>Foundations of Physics III</t>
+  </si>
+  <si>
+    <t>CH</t>
+  </si>
+  <si>
+    <t>General Chemistry I</t>
+  </si>
+  <si>
+    <t>Chemistry</t>
+  </si>
+  <si>
+    <t>General Chemistry II</t>
+  </si>
+  <si>
+    <t>General Chemistry III</t>
+  </si>
+  <si>
+    <t>GEOG</t>
+  </si>
+  <si>
+    <t>The Natural Environment</t>
+  </si>
+  <si>
+    <t>Geography, Climatology, Biology, Geology</t>
+  </si>
+  <si>
+    <t>Climatology</t>
+  </si>
+  <si>
+    <t>Geography, Climatology</t>
+  </si>
+  <si>
+    <t>Geomorphology</t>
+  </si>
+  <si>
+    <t>Geography, Geology</t>
+  </si>
+  <si>
+    <t>Biogeography</t>
+  </si>
+  <si>
+    <t>Geography, Biology</t>
+  </si>
+  <si>
+    <t>GEOL</t>
+  </si>
+  <si>
+    <t>Earth's Interior Heat and Dynamics</t>
+  </si>
+  <si>
+    <t>Geology</t>
+  </si>
+  <si>
+    <t>Earth Surface and Environmental Geology</t>
+  </si>
+  <si>
+    <t>Evolution of the Earth</t>
+  </si>
+  <si>
+    <t>PSY</t>
+  </si>
+  <si>
+    <t>Mind and Brain</t>
+  </si>
+  <si>
+    <t>Psychology</t>
+  </si>
+  <si>
+    <t>Music and the Brain</t>
+  </si>
+  <si>
+    <t>Music, Psychology</t>
+  </si>
+  <si>
+    <t>Scientific Thinking</t>
+  </si>
+  <si>
+    <t>Biopsychology</t>
+  </si>
+  <si>
+    <t>Psychology, Biology</t>
+  </si>
+  <si>
+    <t>Cognition</t>
+  </si>
+  <si>
+    <t>Introduction to Chemical Principles</t>
+  </si>
+  <si>
+    <t>The Chemistry of Sustainability</t>
+  </si>
+  <si>
+    <t>cant find</t>
+  </si>
+  <si>
+    <t>BI</t>
+  </si>
+  <si>
+    <t>General Biology I</t>
+  </si>
+  <si>
+    <t>General Biology II</t>
+  </si>
+  <si>
+    <t>General Biology III</t>
+  </si>
+  <si>
+    <t>WR</t>
+  </si>
+  <si>
+    <t>Composition II</t>
+  </si>
+  <si>
+    <t>Scientific and Technical Writing</t>
+  </si>
+  <si>
+    <t>Business Comunications</t>
+  </si>
+  <si>
+    <t>Business</t>
+  </si>
+  <si>
+    <t>Calculus III</t>
+  </si>
+  <si>
+    <t>Calculus</t>
+  </si>
+  <si>
+    <t>csmath</t>
+  </si>
+  <si>
+    <t>Several-Variable Calculus I</t>
+  </si>
+  <si>
+    <t>Introduction to Differential Equations</t>
+  </si>
+  <si>
+    <t>Several-Variable Calculus II</t>
+  </si>
+  <si>
+    <t>Introduction to Proof</t>
+  </si>
+  <si>
+    <t>Proofs</t>
+  </si>
+  <si>
+    <t>Fundamentals of Analysis I</t>
+  </si>
+  <si>
+    <t>Fundamentals of Analysis II</t>
+  </si>
+  <si>
+    <t>Theory of Differential Equations</t>
+  </si>
+  <si>
+    <t>Probability and Statistics for Data Science</t>
+  </si>
+  <si>
+    <t>Fundamentals of Number Theory I</t>
+  </si>
+  <si>
+    <t>Fundamentals of Number Theory II</t>
+  </si>
+  <si>
+    <t>Elementary Numerical Analysis I</t>
+  </si>
+  <si>
+    <t>Elementary Numerical Analysis II</t>
+  </si>
+  <si>
+    <t>Fundamentals of Abstract Algebra I</t>
+  </si>
+  <si>
+    <t>Fundamentals of Abstract Algebra II</t>
+  </si>
+  <si>
+    <t>Geometries from an Advanced Viewpoint I</t>
+  </si>
+  <si>
+    <t>Geometries from an Advanced Viewpoint II</t>
+  </si>
+  <si>
+    <t>History and Applications of Calculus</t>
+  </si>
+  <si>
+    <t>Functions of a Complex Variable I</t>
+  </si>
+  <si>
+    <t>Functions of a Complex Variable II</t>
+  </si>
+  <si>
+    <t>Introduction to Analysis I</t>
+  </si>
+  <si>
+    <t>Introduction to Analysis II</t>
+  </si>
+  <si>
+    <t>Introduction to Analysis III</t>
+  </si>
+  <si>
+    <t>Partial Differential Equations: Fourier Analysis I</t>
+  </si>
+  <si>
+    <t>Partial Differential Equations: Fourier Analysis II</t>
+  </si>
+  <si>
+    <t>Introduction to Topology I</t>
+  </si>
+  <si>
+    <t>Introduction to Topology II</t>
+  </si>
+  <si>
+    <t>Introduction to Differential Geometry</t>
+  </si>
+  <si>
+    <t>Introduction to Topology III</t>
+  </si>
+  <si>
+    <t>Linear Algebra</t>
+  </si>
+  <si>
+    <t>Introduction to Abstract Algebra I</t>
+  </si>
+  <si>
+    <t>Introduction to Abstract Algebra II</t>
+  </si>
+  <si>
+    <t>Introduction to Abstract Algebra III</t>
+  </si>
+  <si>
+    <t>Introduction to Mathematical Methods of Statistics I</t>
+  </si>
+  <si>
+    <t>Introduction to Mathematical Methods of Statistics II</t>
+  </si>
+  <si>
+    <t>Mathematical Methods of Regression Analysis and Analysis of Variance</t>
+  </si>
+  <si>
+    <t>Stochastic Processes</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -307,16 +658,26 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
+    <font>
       <color rgb="FF312B2C"/>
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="lightGray"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -325,17 +686,20 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="3" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -553,6 +917,9 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="8" max="8" width="17.88"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
@@ -585,13 +952,19 @@
       <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1">
-        <v>21000.0</v>
+        <v>210000.0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C2" s="1">
         <v>210.0</v>
@@ -603,343 +976,415 @@
         <v>4.0</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="G2" s="1" t="b">
         <v>1</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="I2" s="1" t="b">
         <v>1</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1">
-        <v>21100.0</v>
+        <v>211000.0</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C3" s="1">
         <v>211.0</v>
       </c>
       <c r="D3" s="1">
-        <v>21000.0</v>
+        <v>210000.0</v>
       </c>
       <c r="E3" s="1">
         <v>4.0</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="G3" s="1" t="b">
         <v>1</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="I3" s="1" t="b">
         <v>1</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1">
-        <v>21200.0</v>
+        <v>212000.0</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C4" s="1">
         <v>212.0</v>
       </c>
       <c r="D4" s="1">
-        <v>21100.0</v>
+        <v>211000.0</v>
       </c>
       <c r="E4" s="1">
         <v>4.0</v>
       </c>
       <c r="F4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I4" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="J4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="G4" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="I4" s="1" t="b">
-        <v>1</v>
+      <c r="K4" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1">
-        <v>31300.0</v>
+        <v>313000.0</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C5" s="1">
         <v>313.0</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>17</v>
+      <c r="D5" s="3" t="s">
+        <v>21</v>
       </c>
       <c r="E5" s="1">
         <v>4.0</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="G5" s="1" t="b">
         <v>1</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="I5" s="1" t="b">
         <v>1</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1">
-        <v>31400.0</v>
+        <v>314000.0</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C6" s="1">
         <v>314.0</v>
       </c>
       <c r="D6" s="1">
-        <v>21200.0</v>
+        <v>212000.0</v>
       </c>
       <c r="E6" s="1">
         <v>4.0</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="G6" s="1" t="b">
         <v>1</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="I6" s="1" t="b">
         <v>1</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1">
-        <v>31500.0</v>
+        <v>315000.0</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C7" s="1">
         <v>315.0</v>
       </c>
       <c r="D7" s="1">
-        <v>31300.0</v>
+        <v>313000.0</v>
       </c>
       <c r="E7" s="1">
         <v>4.0</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="G7" s="1" t="b">
         <v>1</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="I7" s="1" t="b">
         <v>1</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1">
-        <v>33300.0</v>
+        <v>333000.0</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C8" s="1">
         <v>333.0</v>
       </c>
       <c r="D8" s="1">
-        <v>21200.0</v>
+        <v>212000.0</v>
       </c>
       <c r="E8" s="1">
         <v>4.0</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="G8" s="1" t="b">
         <v>1</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="I8" s="1" t="b">
         <v>0</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1">
-        <v>32200.0</v>
+        <v>322000.0</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C9" s="1">
         <v>322.0</v>
       </c>
       <c r="D9" s="1">
-        <v>21200.0</v>
+        <v>212000.0</v>
       </c>
       <c r="E9" s="1">
         <v>4.0</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="G9" s="1" t="b">
         <v>1</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="I9" s="1" t="b">
         <v>0</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1">
-        <v>44300.0</v>
+        <v>443000.0</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C10" s="1">
         <v>443.0</v>
       </c>
       <c r="D10" s="1">
-        <v>31300.0</v>
+        <v>313000.0</v>
       </c>
       <c r="E10" s="1">
         <v>4.0</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="G10" s="1" t="b">
         <v>1</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="I10" s="1" t="b">
         <v>0</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1">
-        <v>45100.0</v>
+        <v>451000.0</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C11" s="1">
         <v>451.0</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="E11" s="1">
         <v>4.0</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="G11" s="1" t="b">
         <v>1</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="I11" s="1" t="b">
         <v>0</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1">
-        <v>45300.0</v>
+        <v>453000.0</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C12" s="1">
         <v>453.0</v>
       </c>
       <c r="D12" s="1">
-        <v>45100.0</v>
+        <v>451000.0</v>
       </c>
       <c r="E12" s="1">
         <v>4.0</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="G12" s="1" t="b">
         <v>0</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="I12" s="1" t="b">
         <v>0</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="K12" s="2" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1">
-        <v>410001.0</v>
+        <v>4100001.0</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C13" s="1">
         <v>410.0</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="E13" s="1">
         <v>4.0</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="G13" s="1" t="b">
         <v>1</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="I13" s="1" t="b">
         <v>0</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="K13" s="2" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1">
-        <v>410002.0</v>
+        <v>4100002.0</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C14" s="1">
         <v>410.0</v>
@@ -948,24 +1393,30 @@
         <v>4.0</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="G14" s="1" t="b">
         <v>1</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="I14" s="1" t="b">
         <v>0</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="K14" s="2" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1">
-        <v>410003.0</v>
+        <v>4100003.0</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C15" s="1">
         <v>410.0</v>
@@ -974,190 +1425,232 @@
         <v>4.0</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="G15" s="1" t="b">
         <v>1</v>
       </c>
       <c r="H15" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="I15" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="K15" s="2" t="s">
         <v>34</v>
-      </c>
-      <c r="I15" s="1" t="b">
-        <v>0</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1">
-        <v>33000.0</v>
+        <v>330000.0</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C16" s="1">
         <v>330.0</v>
       </c>
       <c r="D16" s="1">
-        <v>31400.0</v>
+        <v>314000.0</v>
       </c>
       <c r="E16" s="1">
         <v>4.0</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="G16" s="1" t="b">
         <v>1</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>35</v>
+        <v>49</v>
       </c>
       <c r="I16" s="1" t="b">
         <v>1</v>
+      </c>
+      <c r="J16" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K16" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1">
-        <v>42200.0</v>
+        <v>422000.0</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C17" s="1">
         <v>422.0</v>
       </c>
       <c r="D17" s="1">
-        <v>31300.0</v>
+        <v>313000.0</v>
       </c>
       <c r="E17" s="1">
         <v>4.0</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>36</v>
+        <v>50</v>
       </c>
       <c r="G17" s="1" t="b">
         <v>1</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>37</v>
+        <v>51</v>
       </c>
       <c r="I17" s="1" t="b">
         <v>1</v>
+      </c>
+      <c r="J17" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K17" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1">
-        <v>44100.0</v>
+        <v>441000.0</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C18" s="1">
         <v>441.0</v>
       </c>
       <c r="D18" s="1">
-        <v>33000.0</v>
+        <v>330000.0</v>
       </c>
       <c r="E18" s="1">
         <v>4.0</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="G18" s="1" t="b">
         <v>0</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>38</v>
+        <v>52</v>
       </c>
       <c r="I18" s="1" t="b">
         <v>0</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="K18" s="2" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1">
-        <v>43600.0</v>
+        <v>436000.0</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C19" s="1">
         <v>436.0</v>
       </c>
       <c r="D19" s="1">
-        <v>33000.0</v>
+        <v>330000.0</v>
       </c>
       <c r="E19" s="1">
         <v>4.0</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="G19" s="1" t="b">
         <v>0</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>39</v>
+        <v>54</v>
       </c>
       <c r="I19" s="1" t="b">
         <v>0</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="K19" s="2" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1">
-        <v>43200.0</v>
+        <v>432000.0</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C20" s="1">
         <v>432.0</v>
       </c>
       <c r="D20" s="1">
-        <v>33000.0</v>
+        <v>330000.0</v>
       </c>
       <c r="E20" s="1">
         <v>4.0</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="G20" s="1" t="b">
         <v>1</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>40</v>
+        <v>56</v>
       </c>
       <c r="I20" s="1" t="b">
         <v>0</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="K20" s="2" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1">
-        <v>43100.0</v>
+        <v>431000.0</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C21" s="1">
         <v>431.0</v>
       </c>
       <c r="D21" s="1">
-        <v>33000.0</v>
+        <v>330000.0</v>
       </c>
       <c r="E21" s="1">
         <v>4.0</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="G21" s="1" t="b">
         <v>0</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>41</v>
+        <v>58</v>
       </c>
       <c r="I21" s="1" t="b">
         <v>0</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="K21" s="2" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="22">
@@ -1165,683 +1658,2711 @@
         <v>429000.0</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C22" s="1">
         <v>429.0</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>42</v>
+        <v>60</v>
       </c>
       <c r="E22" s="1">
         <v>4.0</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="G22" s="1" t="b">
         <v>0</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>43</v>
+        <v>61</v>
       </c>
       <c r="I22" s="1" t="b">
         <v>0</v>
+      </c>
+      <c r="J22" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="K22" s="2" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1">
-        <v>44500.0</v>
+        <v>445000.0</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C23" s="1">
         <v>445.0</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>44</v>
+        <v>63</v>
       </c>
       <c r="E23" s="1">
         <v>4.0</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="G23" s="1" t="b">
         <v>0</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>45</v>
+        <v>64</v>
       </c>
       <c r="I23" s="1" t="b">
         <v>0</v>
+      </c>
+      <c r="J23" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="K23" s="2" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1">
-        <v>41500.0</v>
+        <v>415000.0</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C24" s="1">
         <v>415.0</v>
       </c>
       <c r="D24" s="1">
-        <v>33000.0</v>
+        <v>330000.0</v>
       </c>
       <c r="E24" s="1">
         <v>4.0</v>
       </c>
       <c r="F24" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G24" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="I24" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="J24" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="G24" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="H24" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="I24" s="1" t="b">
-        <v>1</v>
+      <c r="K24" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1">
-        <v>47100.0</v>
+        <v>471000.0</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C25" s="1">
         <v>471.0</v>
       </c>
       <c r="D25" s="1">
-        <v>31500.0</v>
+        <v>315000.0</v>
       </c>
       <c r="E25" s="1">
         <v>4.0</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="G25" s="1" t="b">
         <v>1</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>47</v>
+        <v>66</v>
       </c>
       <c r="I25" s="1" t="b">
         <v>0</v>
+      </c>
+      <c r="J25" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="K25" s="2" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1">
-        <v>47200.0</v>
+        <v>472000.0</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C26" s="1">
         <v>472.0</v>
       </c>
       <c r="D26" s="1">
-        <v>31500.0</v>
+        <v>315000.0</v>
       </c>
       <c r="E26" s="1">
         <v>4.0</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="G26" s="1" t="b">
         <v>1</v>
       </c>
       <c r="H26" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="I26" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="J26" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="I26" s="1" t="b">
-        <v>0</v>
+      <c r="K26" s="2" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1">
-        <v>42500.0</v>
+        <v>425000.0</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C27" s="1">
         <v>425.0</v>
       </c>
       <c r="D27" s="1">
-        <v>31500.0</v>
+        <v>315000.0</v>
       </c>
       <c r="E27" s="1">
         <v>4.0</v>
       </c>
       <c r="F27" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G27" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I27" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="J27" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="G27" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="H27" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="I27" s="1" t="b">
-        <v>1</v>
+      <c r="K27" s="2" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1">
-        <v>41300.0</v>
+        <v>413000.0</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C28" s="1">
         <v>413.0</v>
       </c>
       <c r="D28" s="1">
-        <v>31500.0</v>
+        <v>315000.0</v>
       </c>
       <c r="E28" s="1">
         <v>4.0</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="G28" s="1" t="b">
         <v>1</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>50</v>
+        <v>69</v>
       </c>
       <c r="I28" s="1" t="b">
         <v>0</v>
+      </c>
+      <c r="J28" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="K28" s="1" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1">
-        <v>42000.0</v>
+        <v>420000.0</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C29" s="1">
         <v>420.0</v>
       </c>
       <c r="D29" s="1">
-        <v>31500.0</v>
+        <v>315000.0</v>
       </c>
       <c r="E29" s="1">
         <v>4.0</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="G29" s="1" t="b">
         <v>0</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>51</v>
+        <v>71</v>
       </c>
       <c r="I29" s="1" t="b">
         <v>0</v>
+      </c>
+      <c r="J29" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="K29" s="1" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1">
-        <v>47300.0</v>
+        <v>427000.0</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C30" s="1">
-        <v>473.0</v>
-      </c>
-      <c r="D30" s="1">
-        <v>31500.0</v>
-      </c>
+        <v>427.0</v>
+      </c>
+      <c r="D30" s="1"/>
       <c r="E30" s="1">
         <v>4.0</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="G30" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="H30" s="1" t="s">
-        <v>52</v>
-      </c>
+      <c r="H30" s="1"/>
       <c r="I30" s="1" t="b">
         <v>0</v>
+      </c>
+      <c r="J30" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K30" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="L30" s="1" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1">
-        <v>42300.0</v>
+        <v>473000.0</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C31" s="1">
-        <v>423.0</v>
+        <v>473.0</v>
       </c>
       <c r="D31" s="1">
-        <v>42200.0</v>
+        <v>315000.0</v>
       </c>
       <c r="E31" s="1">
         <v>4.0</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="G31" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>53</v>
+        <v>73</v>
       </c>
       <c r="I31" s="1" t="b">
         <v>0</v>
+      </c>
+      <c r="J31" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="K31" s="1" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1">
-        <v>46100.0</v>
+        <v>423000.0</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C32" s="1">
-        <v>461.0</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>54</v>
+        <v>423.0</v>
+      </c>
+      <c r="D32" s="1">
+        <v>422000.0</v>
       </c>
       <c r="E32" s="1">
         <v>4.0</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="G32" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>55</v>
+        <v>74</v>
       </c>
       <c r="I32" s="1" t="b">
         <v>0</v>
+      </c>
+      <c r="J32" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="K32" s="2" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1">
-        <v>43300.0</v>
+        <v>461000.0</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C33" s="1">
-        <v>433.0</v>
-      </c>
-      <c r="D33" s="1">
-        <v>41500.0</v>
+        <v>461.0</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>76</v>
       </c>
       <c r="E33" s="1">
         <v>4.0</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="G33" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>56</v>
+        <v>77</v>
       </c>
       <c r="I33" s="1" t="b">
         <v>0</v>
+      </c>
+      <c r="J33" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="K33" s="2" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="1">
-        <v>43400.0</v>
+        <v>433000.0</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C34" s="1">
-        <v>434.0</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>57</v>
+        <v>433.0</v>
+      </c>
+      <c r="D34" s="1">
+        <v>415000.0</v>
       </c>
       <c r="E34" s="1">
         <v>4.0</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>28</v>
+        <v>44</v>
       </c>
       <c r="G34" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>58</v>
+        <v>78</v>
       </c>
       <c r="I34" s="1" t="b">
         <v>0</v>
+      </c>
+      <c r="J34" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="K34" s="2" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="1">
-        <v>23101.0</v>
+        <v>434000.0</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>59</v>
+        <v>12</v>
       </c>
       <c r="C35" s="1">
-        <v>231.0</v>
-      </c>
-      <c r="D35" s="1">
-        <v>11201.0</v>
+        <v>434.0</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>80</v>
       </c>
       <c r="E35" s="1">
         <v>4.0</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="G35" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>60</v>
+        <v>81</v>
       </c>
       <c r="I35" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="J35" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="K35" s="2" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1">
-        <v>23201.0</v>
+        <v>112001.0</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>59</v>
+        <v>82</v>
       </c>
       <c r="C36" s="1">
-        <v>232.0</v>
-      </c>
-      <c r="D36" s="1">
-        <v>23101.0</v>
-      </c>
+        <v>112.0</v>
+      </c>
+      <c r="D36" s="1"/>
       <c r="E36" s="1">
         <v>4.0</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>36</v>
+        <v>50</v>
       </c>
       <c r="G36" s="1" t="b">
         <v>1</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>61</v>
+        <v>83</v>
       </c>
       <c r="I36" s="1" t="b">
         <v>1</v>
+      </c>
+      <c r="J36" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K36" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="1">
-        <v>25101.0</v>
+        <v>231001.0</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>59</v>
+        <v>82</v>
       </c>
       <c r="C37" s="1">
-        <v>251.0</v>
+        <v>231.0</v>
       </c>
       <c r="D37" s="1">
-        <v>11201.0</v>
+        <v>112001.0</v>
       </c>
       <c r="E37" s="1">
         <v>4.0</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>36</v>
+        <v>50</v>
       </c>
       <c r="G37" s="1" t="b">
         <v>1</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>62</v>
+        <v>84</v>
       </c>
       <c r="I37" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="J37" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K37" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="1">
-        <v>25201.0</v>
+        <v>232001.0</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>59</v>
+        <v>82</v>
       </c>
       <c r="C38" s="1">
-        <v>252.0</v>
+        <v>232.0</v>
       </c>
       <c r="D38" s="1">
-        <v>25101.0</v>
+        <v>231001.0</v>
       </c>
       <c r="E38" s="1">
         <v>4.0</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>36</v>
+        <v>50</v>
       </c>
       <c r="G38" s="1" t="b">
         <v>1</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>63</v>
+        <v>85</v>
       </c>
       <c r="I38" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="J38" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K38" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="1">
-        <v>34301.0</v>
+        <v>251001.0</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>59</v>
+        <v>82</v>
       </c>
       <c r="C39" s="1">
-        <v>343.0</v>
+        <v>251.0</v>
       </c>
       <c r="D39" s="1">
-        <v>25201.0</v>
+        <v>112001.0</v>
       </c>
       <c r="E39" s="1">
         <v>4.0</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>13</v>
+        <v>50</v>
       </c>
       <c r="G39" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="H39" s="3" t="s">
-        <v>64</v>
+      <c r="H39" s="1" t="s">
+        <v>86</v>
       </c>
       <c r="I39" s="1" t="b">
         <v>0</v>
+      </c>
+      <c r="J39" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K39" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="L39" s="1" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="1">
-        <v>34101.0</v>
+        <v>252001.0</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>59</v>
+        <v>82</v>
       </c>
       <c r="C40" s="1">
-        <v>341.0</v>
+        <v>252.0</v>
       </c>
       <c r="D40" s="1">
-        <v>25201.0</v>
+        <v>251001.0</v>
       </c>
       <c r="E40" s="1">
         <v>4.0</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>11</v>
+        <v>50</v>
       </c>
       <c r="G40" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="H40" s="3" t="s">
-        <v>65</v>
+      <c r="H40" s="1" t="s">
+        <v>88</v>
       </c>
       <c r="I40" s="1" t="b">
         <v>0</v>
+      </c>
+      <c r="J40" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K40" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="1">
-        <v>34201.0</v>
+        <v>343001.0</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>59</v>
+        <v>82</v>
       </c>
       <c r="C41" s="1">
-        <v>342.0</v>
+        <v>343.0</v>
       </c>
       <c r="D41" s="1">
-        <v>34101.0</v>
+        <v>252001.0</v>
       </c>
       <c r="E41" s="1">
         <v>4.0</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="G41" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="H41" s="3" t="s">
-        <v>66</v>
+      <c r="H41" s="4" t="s">
+        <v>89</v>
       </c>
       <c r="I41" s="1" t="b">
         <v>0</v>
+      </c>
+      <c r="J41" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="K41" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="1">
-        <v>24601.0</v>
+        <v>341001.0</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>59</v>
+        <v>82</v>
       </c>
       <c r="C42" s="1">
-        <v>246.0</v>
+        <v>341.0</v>
       </c>
       <c r="D42" s="1">
-        <v>11201.0</v>
+        <v>252001.0</v>
       </c>
       <c r="E42" s="1">
         <v>4.0</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="G42" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="H42" s="1" t="s">
-        <v>67</v>
+      <c r="H42" s="4" t="s">
+        <v>91</v>
       </c>
       <c r="I42" s="1" t="b">
         <v>0</v>
+      </c>
+      <c r="J42" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="K42" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="1">
-        <v>24701.0</v>
+        <v>342001.0</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>59</v>
+        <v>82</v>
       </c>
       <c r="C43" s="1">
-        <v>247.0</v>
+        <v>342.0</v>
       </c>
       <c r="D43" s="1">
-        <v>24601.0</v>
+        <v>341001.0</v>
       </c>
       <c r="E43" s="1">
         <v>4.0</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="G43" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="H43" s="1" t="s">
-        <v>68</v>
+      <c r="H43" s="4" t="s">
+        <v>92</v>
       </c>
       <c r="I43" s="1" t="b">
         <v>0</v>
+      </c>
+      <c r="J43" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="K43" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="1">
-        <v>26101.0</v>
+        <v>246001.0</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>59</v>
+        <v>82</v>
       </c>
       <c r="C44" s="1">
-        <v>261.0</v>
+        <v>246.0</v>
+      </c>
+      <c r="D44" s="1">
+        <v>112001.0</v>
       </c>
       <c r="E44" s="1">
         <v>4.0</v>
       </c>
+      <c r="F44" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="G44" s="1" t="b">
         <v>1</v>
       </c>
       <c r="H44" s="1" t="s">
-        <v>69</v>
+        <v>93</v>
       </c>
       <c r="I44" s="1" t="b">
         <v>0</v>
+      </c>
+      <c r="J44" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="K44" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="1">
-        <v>26201.0</v>
+        <v>247001.0</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>59</v>
+        <v>82</v>
       </c>
       <c r="C45" s="1">
+        <v>247.0</v>
+      </c>
+      <c r="D45" s="1">
+        <v>246001.0</v>
+      </c>
+      <c r="E45" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G45" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="H45" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="I45" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="J45" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="K45" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="1">
+        <v>261001.0</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C46" s="1">
+        <v>261.0</v>
+      </c>
+      <c r="E46" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G46" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="H46" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="I46" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="J46" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K46" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="L46" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="1">
+        <v>262001.0</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C47" s="1">
         <v>262.0</v>
       </c>
-      <c r="E45" s="1">
-        <v>4.0</v>
-      </c>
-      <c r="G45" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="H45" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="I45" s="1" t="b">
-        <v>0</v>
+      <c r="E47" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G47" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="H47" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="I47" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="J47" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K47" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="1">
+        <v>201002.0</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C48" s="1">
+        <v>201.0</v>
+      </c>
+      <c r="E48" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="H48" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="I48" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="J48" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="K48" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="1">
+        <v>202002.0</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C49" s="1">
+        <v>202.0</v>
+      </c>
+      <c r="E49" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="H49" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="I49" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="J49" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="K49" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="1">
+        <v>203002.0</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C50" s="1">
+        <v>203.0</v>
+      </c>
+      <c r="E50" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="H50" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="I50" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="J50" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="K50" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="1">
+        <v>251002.0</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C51" s="1">
+        <v>251.0</v>
+      </c>
+      <c r="E51" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="H51" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="I51" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="J51" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="K51" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="1">
+        <v>252002.0</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C52" s="1">
+        <v>252.0</v>
+      </c>
+      <c r="E52" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="H52" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="I52" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="J52" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="K52" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="1">
+        <v>253002.0</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C53" s="1">
+        <v>253.0</v>
+      </c>
+      <c r="E53" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="H53" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="I53" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="J53" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="K53" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="1">
+        <v>221003.0</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C54" s="1">
+        <v>221.0</v>
+      </c>
+      <c r="E54" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="H54" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="I54" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="J54" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="K54" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="1">
+        <v>222003.0</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C55" s="1">
+        <v>222.0</v>
+      </c>
+      <c r="E55" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="H55" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="I55" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="J55" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="K55" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="1">
+        <v>223003.0</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C56" s="1">
+        <v>223.0</v>
+      </c>
+      <c r="E56" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="H56" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="I56" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="J56" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="K56" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="1">
+        <v>141004.0</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C57" s="1">
+        <v>141.0</v>
+      </c>
+      <c r="E57" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="H57" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="I57" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="J57" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="K57" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="1">
+        <v>321004.0</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C58" s="1">
+        <v>321.0</v>
+      </c>
+      <c r="E58" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="H58" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="I58" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="J58" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="K58" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="1">
+        <v>322004.0</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C59" s="1">
+        <v>322.0</v>
+      </c>
+      <c r="E59" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="H59" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="I59" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="J59" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="K59" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="1">
+        <v>323004.0</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C60" s="1">
+        <v>323.0</v>
+      </c>
+      <c r="E60" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="H60" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="I60" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="J60" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="K60" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="1">
+        <v>201005.0</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C61" s="1">
+        <v>201.0</v>
+      </c>
+      <c r="E61" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="H61" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="I61" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="J61" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="K61" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="1">
+        <v>202005.0</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C62" s="1">
+        <v>202.0</v>
+      </c>
+      <c r="E62" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="H62" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="I62" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="J62" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="K62" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="1">
+        <v>203005.0</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C63" s="1">
+        <v>203.0</v>
+      </c>
+      <c r="E63" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="H63" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="I63" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="J63" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="K63" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="1">
+        <v>201006.0</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C64" s="1">
+        <v>201.0</v>
+      </c>
+      <c r="E64" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="H64" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="I64" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="J64" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="K64" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="1">
+        <v>348006.0</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C65" s="1">
+        <v>348.0</v>
+      </c>
+      <c r="E65" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="H65" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="I65" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="J65" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="K65" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="1">
+        <v>301006.0</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C66" s="1">
+        <v>301.0</v>
+      </c>
+      <c r="E66" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="H66" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="I66" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="J66" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="K66" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="1">
+        <v>304006.0</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C67" s="1">
+        <v>304.0</v>
+      </c>
+      <c r="E67" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="H67" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="I67" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="J67" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="K67" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="1">
+        <v>305006.0</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C68" s="1">
+        <v>305.0</v>
+      </c>
+      <c r="E68" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="H68" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="I68" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="J68" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="K68" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="1">
+        <v>111003.0</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C69" s="1">
+        <v>111.0</v>
+      </c>
+      <c r="E69" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="H69" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="I69" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="J69" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="K69" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="1">
+        <v>113003.0</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C70" s="1">
+        <v>113.0</v>
+      </c>
+      <c r="E70" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="F70" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H70" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="I70" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="J70" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K70" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="L70" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" s="1">
+        <v>211007.0</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="C71" s="1">
+        <v>211.0</v>
+      </c>
+      <c r="E71" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="H71" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="I71" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="J71" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="K71" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="1">
+        <v>212007.0</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="C72" s="1">
+        <v>212.0</v>
+      </c>
+      <c r="E72" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="H72" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="I72" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="J72" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="K72" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" s="1">
+        <v>213007.0</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="C73" s="1">
+        <v>213.0</v>
+      </c>
+      <c r="E73" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="H73" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="I73" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="J73" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="K73" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" s="1">
+        <v>121008.0</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="C74" s="1">
+        <v>121.0</v>
+      </c>
+      <c r="D74" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E74" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="G74" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="H74" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="I74" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="J74" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K74" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" s="1">
+        <v>122008.0</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="C75" s="1">
+        <v>122.0</v>
+      </c>
+      <c r="D75" s="1">
+        <v>121008.0</v>
+      </c>
+      <c r="E75" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="G75" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="H75" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="I75" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="J75" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K75" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" s="1">
+        <v>320008.0</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="C76" s="1">
+        <v>320.0</v>
+      </c>
+      <c r="D76" s="1">
+        <v>122008.0</v>
+      </c>
+      <c r="E76" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="G76" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="H76" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="I76" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="J76" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K76" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" s="1">
+        <v>321008.0</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="C77" s="1">
+        <v>321.0</v>
+      </c>
+      <c r="D77" s="1">
+        <v>122008.0</v>
+      </c>
+      <c r="E77" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="G77" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="H77" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="I77" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="J77" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="K77" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" s="1">
+        <v>253001.0</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C78" s="1">
+        <v>253.0</v>
+      </c>
+      <c r="D78" s="1">
+        <v>252001.0</v>
+      </c>
+      <c r="E78" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="G78" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="H78" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="I78" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="J78" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="K78" s="1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" s="1">
+        <v>281001.0</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C79" s="1">
+        <v>281.0</v>
+      </c>
+      <c r="D79" s="1">
+        <v>253001.0</v>
+      </c>
+      <c r="E79" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="H79" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="I79" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="J79" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="K79" s="1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" s="1">
+        <v>256001.0</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C80" s="1">
+        <v>256.0</v>
+      </c>
+      <c r="D80" s="1">
+        <v>253001.0</v>
+      </c>
+      <c r="E80" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="H80" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="I80" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="J80" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="K80" s="1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" s="1">
+        <v>282001.0</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C81" s="1">
+        <v>282.0</v>
+      </c>
+      <c r="D81" s="1">
+        <v>281001.0</v>
+      </c>
+      <c r="E81" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="H81" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="I81" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="J81" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="K81" s="1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" s="1">
+        <v>307001.0</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C82" s="1">
+        <v>307.0</v>
+      </c>
+      <c r="D82" s="1">
+        <v>252001.0</v>
+      </c>
+      <c r="E82" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="H82" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="I82" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="J82" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="K82" s="1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" s="1">
+        <v>316001.0</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C83" s="1">
+        <v>316.0</v>
+      </c>
+      <c r="E83" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="H83" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="I83" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="J83" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="K83" s="1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" s="1">
+        <v>317001.0</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C84" s="1">
+        <v>317.0</v>
+      </c>
+      <c r="D84" s="1">
+        <v>316001.0</v>
+      </c>
+      <c r="E84" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="H84" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="I84" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="J84" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="K84" s="1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" s="1">
+        <v>320001.0</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C85" s="1">
+        <v>320.0</v>
+      </c>
+      <c r="E85" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="H85" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="I85" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="J85" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="K85" s="1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" s="1">
+        <v>345001.0</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C86" s="1">
+        <v>345.0</v>
+      </c>
+      <c r="E86" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="H86" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="I86" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="J86" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="K86" s="1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" s="1">
+        <v>347001.0</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C87" s="1">
+        <v>347.0</v>
+      </c>
+      <c r="E87" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="H87" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="I87" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="J87" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="K87" s="1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" s="1">
+        <v>348001.0</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C88" s="1">
+        <v>348.0</v>
+      </c>
+      <c r="D88" s="1">
+        <v>347001.0</v>
+      </c>
+      <c r="E88" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="H88" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="I88" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="J88" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="K88" s="1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" s="1">
+        <v>351001.0</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C89" s="1">
+        <v>351.0</v>
+      </c>
+      <c r="E89" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="H89" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="I89" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="J89" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="K89" s="1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" s="1">
+        <v>352001.0</v>
+      </c>
+      <c r="B90" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C90" s="1">
+        <v>352.0</v>
+      </c>
+      <c r="D90" s="1">
+        <v>351001.0</v>
+      </c>
+      <c r="E90" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="H90" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="I90" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="J90" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="K90" s="1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" s="1">
+        <v>391001.0</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C91" s="1">
+        <v>391.0</v>
+      </c>
+      <c r="E91" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="H91" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="I91" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="J91" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="K91" s="1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" s="1">
+        <v>392001.0</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C92" s="1">
+        <v>392.0</v>
+      </c>
+      <c r="D92" s="1">
+        <v>391001.0</v>
+      </c>
+      <c r="E92" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="H92" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="I92" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="J92" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="K92" s="1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" s="1">
+        <v>394001.0</v>
+      </c>
+      <c r="B93" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C93" s="1">
+        <v>394.0</v>
+      </c>
+      <c r="E93" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="H93" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="I93" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="J93" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="K93" s="1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" s="1">
+        <v>395001.0</v>
+      </c>
+      <c r="B94" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C94" s="1">
+        <v>395.0</v>
+      </c>
+      <c r="D94" s="1">
+        <v>394001.0</v>
+      </c>
+      <c r="E94" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="H94" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="I94" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="J94" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="K94" s="1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" s="1">
+        <v>397001.0</v>
+      </c>
+      <c r="B95" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C95" s="1">
+        <v>397.0</v>
+      </c>
+      <c r="E95" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="H95" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="I95" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="J95" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="K95" s="1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" s="1">
+        <v>411001.0</v>
+      </c>
+      <c r="B96" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C96" s="1">
+        <v>411.0</v>
+      </c>
+      <c r="E96" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="H96" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="I96" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="J96" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="K96" s="1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" s="1">
+        <v>412001.0</v>
+      </c>
+      <c r="B97" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C97" s="1">
+        <v>412.0</v>
+      </c>
+      <c r="E97" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="H97" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="I97" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="J97" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="K97" s="1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" s="1">
+        <v>413001.0</v>
+      </c>
+      <c r="B98" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C98" s="1">
+        <v>413.0</v>
+      </c>
+      <c r="E98" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="H98" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="I98" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="J98" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="K98" s="1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" s="1">
+        <v>414001.0</v>
+      </c>
+      <c r="B99" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C99" s="1">
+        <v>414.0</v>
+      </c>
+      <c r="E99" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="H99" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="I99" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="J99" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="K99" s="1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" s="1">
+        <v>415001.0</v>
+      </c>
+      <c r="B100" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C100" s="1">
+        <v>415.0</v>
+      </c>
+      <c r="E100" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="H100" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="I100" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="J100" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="K100" s="1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" s="1">
+        <v>421001.0</v>
+      </c>
+      <c r="B101" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C101" s="1">
+        <v>421.0</v>
+      </c>
+      <c r="E101" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="H101" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="I101" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="J101" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="K101" s="1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" s="1">
+        <v>422001.0</v>
+      </c>
+      <c r="B102" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C102" s="1">
+        <v>422.0</v>
+      </c>
+      <c r="E102" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="H102" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="I102" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="J102" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="K102" s="1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" s="1">
+        <v>431001.0</v>
+      </c>
+      <c r="B103" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C103" s="1">
+        <v>431.0</v>
+      </c>
+      <c r="E103" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="H103" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="I103" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="J103" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="K103" s="1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" s="1">
+        <v>432001.0</v>
+      </c>
+      <c r="B104" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C104" s="1">
+        <v>432.0</v>
+      </c>
+      <c r="E104" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="H104" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="I104" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="J104" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="K104" s="1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" s="1">
+        <v>433001.0</v>
+      </c>
+      <c r="B105" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C105" s="1">
+        <v>433.0</v>
+      </c>
+      <c r="E105" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="H105" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="I105" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="J105" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="K105" s="1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" s="1">
+        <v>434001.0</v>
+      </c>
+      <c r="B106" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C106" s="1">
+        <v>434.0</v>
+      </c>
+      <c r="E106" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="H106" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="I106" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="J106" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="K106" s="1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" s="1">
+        <v>441001.0</v>
+      </c>
+      <c r="B107" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C107" s="1">
+        <v>441.0</v>
+      </c>
+      <c r="E107" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="H107" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="I107" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="J107" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="K107" s="1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" s="1">
+        <v>444001.0</v>
+      </c>
+      <c r="B108" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C108" s="1">
+        <v>444.0</v>
+      </c>
+      <c r="E108" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="H108" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="I108" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="J108" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="K108" s="1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" s="1">
+        <v>445001.0</v>
+      </c>
+      <c r="B109" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C109" s="1">
+        <v>445.0</v>
+      </c>
+      <c r="E109" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="H109" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="I109" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="J109" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="K109" s="1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" s="1">
+        <v>446001.0</v>
+      </c>
+      <c r="B110" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C110" s="1">
+        <v>446.0</v>
+      </c>
+      <c r="E110" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="H110" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="I110" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="J110" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="K110" s="1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" s="1">
+        <v>461001.0</v>
+      </c>
+      <c r="B111" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C111" s="1">
+        <v>461.0</v>
+      </c>
+      <c r="E111" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="H111" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="I111" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="J111" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="K111" s="1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" s="1">
+        <v>462001.0</v>
+      </c>
+      <c r="B112" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C112" s="1">
+        <v>462.0</v>
+      </c>
+      <c r="E112" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="H112" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="I112" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="J112" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="K112" s="1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" s="1">
+        <v>463001.0</v>
+      </c>
+      <c r="B113" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C113" s="1">
+        <v>463.0</v>
+      </c>
+      <c r="E113" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="H113" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="I113" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="J113" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="K113" s="1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" s="1">
+        <v>467001.0</v>
+      </c>
+      <c r="B114" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C114" s="1">
+        <v>467.0</v>
+      </c>
+      <c r="E114" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="H114" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="I114" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="J114" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="K114" s="1" t="s">
+        <v>150</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add working(?) forecast algorithm to coursestest.py
</commit_message>
<xml_diff>
--- a/cs_degree_planner/forecast/recommendcourses.xlsx
+++ b/cs_degree_planner/forecast/recommendcourses.xlsx
@@ -75,7 +75,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="521" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="641" uniqueCount="205">
   <si>
     <t>id</t>
   </si>
@@ -110,7 +110,7 @@
     <t>satisfyarea</t>
   </si>
   <si>
-    <t>notes</t>
+    <t>miscnotes</t>
   </si>
   <si>
     <t>CS</t>
@@ -128,6 +128,9 @@
     <t>na</t>
   </si>
   <si>
+    <t>todo variable credit</t>
+  </si>
+  <si>
     <t>WS</t>
   </si>
   <si>
@@ -389,27 +392,42 @@
     <t>General Physics III</t>
   </si>
   <si>
+    <t>251001, 112001</t>
+  </si>
+  <si>
     <t>Foundations of Physics I</t>
   </si>
   <si>
     <t>Physics, Advanced Physics</t>
   </si>
   <si>
+    <t>252001, 251002</t>
+  </si>
+  <si>
     <t>Foundations of Physics II</t>
   </si>
   <si>
+    <t>253001, 252002</t>
+  </si>
+  <si>
     <t>Foundations of Physics III</t>
   </si>
   <si>
     <t>CH</t>
   </si>
   <si>
+    <t>111003, 112001</t>
+  </si>
+  <si>
     <t>General Chemistry I</t>
   </si>
   <si>
     <t>Chemistry</t>
   </si>
   <si>
+    <t>112001, 221003</t>
+  </si>
+  <si>
     <t>General Chemistry II</t>
   </si>
   <si>
@@ -443,19 +461,19 @@
     <t>Geography, Biology</t>
   </si>
   <si>
-    <t>GEOL</t>
-  </si>
-  <si>
-    <t>Earth's Interior Heat and Dynamics</t>
-  </si>
-  <si>
-    <t>Geology</t>
+    <t>ERTH</t>
+  </si>
+  <si>
+    <t>Dynamic Planet Earth</t>
+  </si>
+  <si>
+    <t>Earth Sciences, Geology</t>
   </si>
   <si>
     <t>Earth Surface and Environmental Geology</t>
   </si>
   <si>
-    <t>Evolution of the Earth</t>
+    <t>History of Life</t>
   </si>
   <si>
     <t>PSY</t>
@@ -473,6 +491,9 @@
     <t>Music, Psychology</t>
   </si>
   <si>
+    <t>cant find</t>
+  </si>
+  <si>
     <t>Scientific Thinking</t>
   </si>
   <si>
@@ -491,19 +512,16 @@
     <t>The Chemistry of Sustainability</t>
   </si>
   <si>
-    <t>cant find</t>
-  </si>
-  <si>
     <t>BI</t>
   </si>
   <si>
-    <t>General Biology I</t>
-  </si>
-  <si>
-    <t>General Biology II</t>
-  </si>
-  <si>
-    <t>General Biology III</t>
+    <t>General Biology I: Cells</t>
+  </si>
+  <si>
+    <t>General Biology II: Organisms</t>
+  </si>
+  <si>
+    <t>General Biology III: Populations</t>
   </si>
   <si>
     <t>WR</t>
@@ -515,6 +533,9 @@
     <t>Scientific and Technical Writing</t>
   </si>
   <si>
+    <t>req junior standing</t>
+  </si>
+  <si>
     <t>Business Comunications</t>
   </si>
   <si>
@@ -545,15 +566,30 @@
     <t>Proofs</t>
   </si>
   <si>
+    <t>the below math term offerings are just 2022-2023 and not necessarily reflective of general patterns</t>
+  </si>
+  <si>
+    <t>253001, 232001</t>
+  </si>
+  <si>
     <t>Fundamentals of Analysis I</t>
   </si>
   <si>
     <t>Fundamentals of Analysis II</t>
   </si>
   <si>
+    <t>342001, 281001, 232001</t>
+  </si>
+  <si>
     <t>Theory of Differential Equations</t>
   </si>
   <si>
+    <t>last time offered=2021S, previously was annual but not sure if it will exist</t>
+  </si>
+  <si>
+    <t>342001, 211000</t>
+  </si>
+  <si>
     <t>Probability and Statistics for Data Science</t>
   </si>
   <si>
@@ -569,6 +605,9 @@
     <t>Elementary Numerical Analysis II</t>
   </si>
   <si>
+    <t>341001, 232001</t>
+  </si>
+  <si>
     <t>Fundamentals of Abstract Algebra I</t>
   </si>
   <si>
@@ -584,6 +623,9 @@
     <t>History and Applications of Calculus</t>
   </si>
   <si>
+    <t>281001, 232001</t>
+  </si>
+  <si>
     <t>Functions of a Complex Variable I</t>
   </si>
   <si>
@@ -639,6 +681,15 @@
   </si>
   <si>
     <t>Stochastic Processes</t>
+  </si>
+  <si>
+    <t>Statistical Methods I</t>
+  </si>
+  <si>
+    <t>College Algebra</t>
+  </si>
+  <si>
+    <t>Foundations of Algebra and Mathematical Modeling</t>
   </si>
 </sst>
 </file>
@@ -969,8 +1020,8 @@
       <c r="C2" s="1">
         <v>210.0</v>
       </c>
-      <c r="D2" s="1" t="b">
-        <v>0</v>
+      <c r="D2" s="1">
+        <v>112001.0</v>
       </c>
       <c r="E2" s="1">
         <v>4.0</v>
@@ -992,6 +1043,9 @@
       </c>
       <c r="K2" s="1" t="s">
         <v>16</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="3">
@@ -1011,13 +1065,13 @@
         <v>4.0</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G3" s="1" t="b">
         <v>1</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I3" s="1" t="b">
         <v>1</v>
@@ -1046,13 +1100,13 @@
         <v>4.0</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G4" s="1" t="b">
         <v>1</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I4" s="1" t="b">
         <v>1</v>
@@ -1075,7 +1129,7 @@
         <v>313.0</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E5" s="1">
         <v>4.0</v>
@@ -1087,7 +1141,7 @@
         <v>1</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I5" s="1" t="b">
         <v>1</v>
@@ -1122,7 +1176,7 @@
         <v>1</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I6" s="1" t="b">
         <v>1</v>
@@ -1151,13 +1205,13 @@
         <v>4.0</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G7" s="1" t="b">
         <v>1</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="I7" s="1" t="b">
         <v>1</v>
@@ -1186,22 +1240,22 @@
         <v>4.0</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G8" s="1" t="b">
         <v>1</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="I8" s="1" t="b">
         <v>0</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="9">
@@ -1221,22 +1275,22 @@
         <v>4.0</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G9" s="1" t="b">
         <v>1</v>
       </c>
       <c r="H9" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I9" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="K9" s="2" t="s">
         <v>29</v>
-      </c>
-      <c r="I9" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="J9" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="K9" s="2" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="10">
@@ -1256,22 +1310,22 @@
         <v>4.0</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G10" s="1" t="b">
         <v>1</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="I10" s="1" t="b">
         <v>0</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11">
@@ -1285,28 +1339,28 @@
         <v>451.0</v>
       </c>
       <c r="D11" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E11" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G11" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="I11" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="K11" s="2" t="s">
         <v>35</v>
-      </c>
-      <c r="E11" s="1">
-        <v>4.0</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="G11" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="I11" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="J11" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="K11" s="2" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="12">
@@ -1326,22 +1380,22 @@
         <v>4.0</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="G12" s="1" t="b">
         <v>0</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="I12" s="1" t="b">
         <v>0</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="13">
@@ -1355,28 +1409,28 @@
         <v>410.0</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E13" s="1">
         <v>4.0</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G13" s="1" t="b">
         <v>1</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I13" s="1" t="b">
         <v>0</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="14">
@@ -1389,26 +1443,29 @@
       <c r="C14" s="1">
         <v>410.0</v>
       </c>
+      <c r="D14" s="1">
+        <v>330000.0</v>
+      </c>
       <c r="E14" s="1">
         <v>4.0</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="G14" s="1" t="b">
         <v>1</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="I14" s="1" t="b">
         <v>0</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="15">
@@ -1421,26 +1478,29 @@
       <c r="C15" s="1">
         <v>410.0</v>
       </c>
+      <c r="D15" s="1">
+        <v>315000.0</v>
+      </c>
       <c r="E15" s="1">
         <v>4.0</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G15" s="1" t="b">
         <v>1</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="I15" s="1" t="b">
         <v>0</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="K15" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="16">
@@ -1460,13 +1520,13 @@
         <v>4.0</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G16" s="1" t="b">
         <v>1</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="I16" s="1" t="b">
         <v>1</v>
@@ -1495,13 +1555,13 @@
         <v>4.0</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="G17" s="1" t="b">
         <v>1</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="I17" s="1" t="b">
         <v>1</v>
@@ -1530,22 +1590,22 @@
         <v>4.0</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G18" s="1" t="b">
         <v>0</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="I18" s="1" t="b">
         <v>0</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="K18" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="19">
@@ -1565,22 +1625,22 @@
         <v>4.0</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="G19" s="1" t="b">
         <v>0</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="I19" s="1" t="b">
         <v>0</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="K19" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="20">
@@ -1600,22 +1660,22 @@
         <v>4.0</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G20" s="1" t="b">
         <v>1</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="I20" s="1" t="b">
         <v>0</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="K20" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="21">
@@ -1635,22 +1695,22 @@
         <v>4.0</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="G21" s="1" t="b">
         <v>0</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="I21" s="1" t="b">
         <v>0</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="K21" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="22">
@@ -1664,28 +1724,28 @@
         <v>429.0</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E22" s="1">
         <v>4.0</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="G22" s="1" t="b">
         <v>0</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="I22" s="1" t="b">
         <v>0</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="K22" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="23">
@@ -1699,28 +1759,28 @@
         <v>445.0</v>
       </c>
       <c r="D23" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E23" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G23" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="I23" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="J23" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="E23" s="1">
-        <v>4.0</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="G23" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="H23" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="I23" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="J23" s="1" t="s">
-        <v>62</v>
-      </c>
       <c r="K23" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="24">
@@ -1740,13 +1800,13 @@
         <v>4.0</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G24" s="1" t="b">
         <v>1</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="I24" s="1" t="b">
         <v>1</v>
@@ -1775,22 +1835,22 @@
         <v>4.0</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G25" s="1" t="b">
         <v>1</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="I25" s="1" t="b">
         <v>0</v>
       </c>
       <c r="J25" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="K25" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="26">
@@ -1810,22 +1870,22 @@
         <v>4.0</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G26" s="1" t="b">
         <v>1</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="I26" s="1" t="b">
         <v>0</v>
       </c>
       <c r="J26" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="K26" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="27">
@@ -1845,13 +1905,13 @@
         <v>4.0</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G27" s="1" t="b">
         <v>1</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="I27" s="1" t="b">
         <v>1</v>
@@ -1880,22 +1940,22 @@
         <v>4.0</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="G28" s="1" t="b">
         <v>1</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="I28" s="1" t="b">
         <v>0</v>
       </c>
       <c r="J28" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="K28" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="29">
@@ -1915,22 +1975,22 @@
         <v>4.0</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="G29" s="1" t="b">
         <v>0</v>
       </c>
       <c r="H29" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="I29" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="J29" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="K29" s="1" t="s">
         <v>71</v>
-      </c>
-      <c r="I29" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="J29" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="K29" s="1" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="30">
@@ -1948,7 +2008,7 @@
         <v>4.0</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="G30" s="1" t="b">
         <v>0</v>
@@ -1961,10 +2021,10 @@
         <v>15</v>
       </c>
       <c r="K30" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="L30" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="31">
@@ -1984,22 +2044,22 @@
         <v>4.0</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="G31" s="1" t="b">
         <v>0</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="I31" s="1" t="b">
         <v>0</v>
       </c>
       <c r="J31" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="K31" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="32">
@@ -2019,22 +2079,22 @@
         <v>4.0</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G32" s="1" t="b">
         <v>1</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="I32" s="1" t="b">
         <v>0</v>
       </c>
       <c r="J32" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="K32" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="33">
@@ -2048,28 +2108,28 @@
         <v>461.0</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E33" s="1">
         <v>4.0</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="G33" s="1" t="b">
         <v>0</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="I33" s="1" t="b">
         <v>0</v>
       </c>
       <c r="J33" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="K33" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="34">
@@ -2089,22 +2149,22 @@
         <v>4.0</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="G34" s="1" t="b">
         <v>1</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="I34" s="1" t="b">
         <v>0</v>
       </c>
       <c r="J34" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="K34" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="35">
@@ -2118,28 +2178,28 @@
         <v>434.0</v>
       </c>
       <c r="D35" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="E35" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G35" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="H35" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="I35" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="J35" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="E35" s="1">
-        <v>4.0</v>
-      </c>
-      <c r="F35" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="G35" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="H35" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="I35" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="J35" s="1" t="s">
-        <v>79</v>
-      </c>
       <c r="K35" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="36">
@@ -2147,23 +2207,25 @@
         <v>112001.0</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C36" s="1">
         <v>112.0</v>
       </c>
-      <c r="D36" s="1"/>
+      <c r="D36" s="1">
+        <v>111001.0</v>
+      </c>
       <c r="E36" s="1">
         <v>4.0</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="G36" s="1" t="b">
         <v>1</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="I36" s="1" t="b">
         <v>1</v>
@@ -2180,7 +2242,7 @@
         <v>231001.0</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C37" s="1">
         <v>231.0</v>
@@ -2192,13 +2254,13 @@
         <v>4.0</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="G37" s="1" t="b">
         <v>1</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="I37" s="1" t="b">
         <v>1</v>
@@ -2215,7 +2277,7 @@
         <v>232001.0</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C38" s="1">
         <v>232.0</v>
@@ -2227,13 +2289,13 @@
         <v>4.0</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="G38" s="1" t="b">
         <v>1</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="I38" s="1" t="b">
         <v>1</v>
@@ -2250,7 +2312,7 @@
         <v>251001.0</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C39" s="1">
         <v>251.0</v>
@@ -2262,13 +2324,13 @@
         <v>4.0</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="G39" s="1" t="b">
         <v>1</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="I39" s="1" t="b">
         <v>0</v>
@@ -2280,7 +2342,7 @@
         <v>16</v>
       </c>
       <c r="L39" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="40">
@@ -2288,7 +2350,7 @@
         <v>252001.0</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C40" s="1">
         <v>252.0</v>
@@ -2300,13 +2362,13 @@
         <v>4.0</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="G40" s="1" t="b">
         <v>1</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="I40" s="1" t="b">
         <v>0</v>
@@ -2323,7 +2385,7 @@
         <v>343001.0</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C41" s="1">
         <v>343.0</v>
@@ -2335,19 +2397,19 @@
         <v>4.0</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G41" s="1" t="b">
         <v>1</v>
       </c>
       <c r="H41" s="4" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="I41" s="1" t="b">
         <v>0</v>
       </c>
       <c r="J41" s="2" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="K41" s="1" t="s">
         <v>16</v>
@@ -2358,7 +2420,7 @@
         <v>341001.0</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C42" s="1">
         <v>341.0</v>
@@ -2376,13 +2438,13 @@
         <v>1</v>
       </c>
       <c r="H42" s="4" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="I42" s="1" t="b">
         <v>0</v>
       </c>
       <c r="J42" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="K42" s="1" t="s">
         <v>16</v>
@@ -2393,7 +2455,7 @@
         <v>342001.0</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C43" s="1">
         <v>342.0</v>
@@ -2405,19 +2467,19 @@
         <v>4.0</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G43" s="1" t="b">
         <v>1</v>
       </c>
       <c r="H43" s="4" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="I43" s="1" t="b">
         <v>0</v>
       </c>
       <c r="J43" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="K43" s="1" t="s">
         <v>16</v>
@@ -2428,7 +2490,7 @@
         <v>246001.0</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C44" s="1">
         <v>246.0</v>
@@ -2446,13 +2508,13 @@
         <v>1</v>
       </c>
       <c r="H44" s="1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="I44" s="1" t="b">
         <v>0</v>
       </c>
       <c r="J44" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="K44" s="1" t="s">
         <v>16</v>
@@ -2463,7 +2525,7 @@
         <v>247001.0</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C45" s="1">
         <v>247.0</v>
@@ -2475,19 +2537,19 @@
         <v>4.0</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G45" s="1" t="b">
         <v>1</v>
       </c>
       <c r="H45" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="I45" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="J45" s="2" t="s">
         <v>95</v>
-      </c>
-      <c r="I45" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="J45" s="2" t="s">
-        <v>94</v>
       </c>
       <c r="K45" s="1" t="s">
         <v>16</v>
@@ -2498,7 +2560,7 @@
         <v>261001.0</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C46" s="1">
         <v>261.0</v>
@@ -2507,13 +2569,13 @@
         <v>4.0</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="G46" s="1" t="b">
         <v>0</v>
       </c>
       <c r="H46" s="1" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="I46" s="1" t="b">
         <v>0</v>
@@ -2525,7 +2587,7 @@
         <v>16</v>
       </c>
       <c r="L46" s="1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="47">
@@ -2533,7 +2595,7 @@
         <v>262001.0</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C47" s="1">
         <v>262.0</v>
@@ -2542,13 +2604,13 @@
         <v>4.0</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="G47" s="1" t="b">
         <v>0</v>
       </c>
       <c r="H47" s="1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="I47" s="1" t="b">
         <v>0</v>
@@ -2565,22 +2627,31 @@
         <v>201002.0</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C48" s="1">
         <v>201.0</v>
       </c>
+      <c r="D48" s="1">
+        <v>112001.0</v>
+      </c>
       <c r="E48" s="1">
         <v>4.0</v>
       </c>
+      <c r="F48" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G48" s="1" t="b">
+        <v>1</v>
+      </c>
       <c r="H48" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="I48" s="1" t="b">
         <v>0</v>
       </c>
       <c r="J48" s="2" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="K48" s="1" t="s">
         <v>16</v>
@@ -2591,22 +2662,31 @@
         <v>202002.0</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C49" s="1">
         <v>202.0</v>
       </c>
+      <c r="D49" s="1">
+        <v>201002.0</v>
+      </c>
       <c r="E49" s="1">
         <v>4.0</v>
       </c>
+      <c r="F49" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G49" s="1" t="b">
+        <v>1</v>
+      </c>
       <c r="H49" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="I49" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="J49" s="2" t="s">
         <v>102</v>
-      </c>
-      <c r="I49" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="J49" s="2" t="s">
-        <v>101</v>
       </c>
       <c r="K49" s="1" t="s">
         <v>16</v>
@@ -2617,22 +2697,31 @@
         <v>203002.0</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C50" s="1">
         <v>203.0</v>
       </c>
+      <c r="D50" s="1">
+        <v>202002.0</v>
+      </c>
       <c r="E50" s="1">
         <v>4.0</v>
       </c>
+      <c r="F50" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G50" s="1" t="b">
+        <v>1</v>
+      </c>
       <c r="H50" s="1" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="I50" s="1" t="b">
         <v>0</v>
       </c>
       <c r="J50" s="2" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="K50" s="1" t="s">
         <v>16</v>
@@ -2643,22 +2732,31 @@
         <v>251002.0</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C51" s="1">
         <v>251.0</v>
       </c>
+      <c r="D51" s="1" t="s">
+        <v>105</v>
+      </c>
       <c r="E51" s="1">
         <v>4.0</v>
       </c>
+      <c r="F51" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G51" s="1" t="b">
+        <v>1</v>
+      </c>
       <c r="H51" s="1" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="I51" s="1" t="b">
         <v>0</v>
       </c>
       <c r="J51" s="2" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="K51" s="1" t="s">
         <v>16</v>
@@ -2669,22 +2767,31 @@
         <v>252002.0</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C52" s="1">
         <v>252.0</v>
       </c>
+      <c r="D52" s="1" t="s">
+        <v>108</v>
+      </c>
       <c r="E52" s="1">
         <v>4.0</v>
       </c>
+      <c r="F52" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G52" s="1" t="b">
+        <v>1</v>
+      </c>
       <c r="H52" s="1" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="I52" s="1" t="b">
         <v>0</v>
       </c>
       <c r="J52" s="2" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="K52" s="1" t="s">
         <v>16</v>
@@ -2695,22 +2802,31 @@
         <v>253002.0</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C53" s="1">
         <v>253.0</v>
       </c>
+      <c r="D53" s="1" t="s">
+        <v>110</v>
+      </c>
       <c r="E53" s="1">
         <v>4.0</v>
       </c>
+      <c r="F53" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G53" s="1" t="b">
+        <v>1</v>
+      </c>
       <c r="H53" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="I53" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="J53" s="2" t="s">
         <v>107</v>
-      </c>
-      <c r="I53" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="J53" s="2" t="s">
-        <v>105</v>
       </c>
       <c r="K53" s="1" t="s">
         <v>16</v>
@@ -2721,22 +2837,31 @@
         <v>221003.0</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="C54" s="1">
         <v>221.0</v>
       </c>
+      <c r="D54" s="1" t="s">
+        <v>113</v>
+      </c>
       <c r="E54" s="1">
         <v>4.0</v>
       </c>
+      <c r="F54" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G54" s="1" t="b">
+        <v>1</v>
+      </c>
       <c r="H54" s="1" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="I54" s="1" t="b">
         <v>0</v>
       </c>
       <c r="J54" s="2" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="K54" s="1" t="s">
         <v>16</v>
@@ -2747,22 +2872,31 @@
         <v>222003.0</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="C55" s="1">
         <v>222.0</v>
       </c>
+      <c r="D55" s="1" t="s">
+        <v>116</v>
+      </c>
       <c r="E55" s="1">
         <v>4.0</v>
       </c>
+      <c r="F55" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G55" s="1" t="b">
+        <v>1</v>
+      </c>
       <c r="H55" s="1" t="s">
-        <v>111</v>
+        <v>117</v>
       </c>
       <c r="I55" s="1" t="b">
         <v>0</v>
       </c>
       <c r="J55" s="2" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="K55" s="1" t="s">
         <v>16</v>
@@ -2773,22 +2907,31 @@
         <v>223003.0</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="C56" s="1">
         <v>223.0</v>
       </c>
+      <c r="D56" s="1">
+        <v>222003.0</v>
+      </c>
       <c r="E56" s="1">
         <v>4.0</v>
       </c>
+      <c r="F56" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G56" s="1" t="b">
+        <v>1</v>
+      </c>
       <c r="H56" s="1" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
       <c r="I56" s="1" t="b">
         <v>0</v>
       </c>
       <c r="J56" s="2" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="K56" s="1" t="s">
         <v>16</v>
@@ -2799,22 +2942,31 @@
         <v>141004.0</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>113</v>
+        <v>119</v>
       </c>
       <c r="C57" s="1">
         <v>141.0</v>
       </c>
+      <c r="D57" s="1" t="b">
+        <v>0</v>
+      </c>
       <c r="E57" s="1">
         <v>4.0</v>
       </c>
+      <c r="F57" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="G57" s="1" t="b">
+        <v>1</v>
+      </c>
       <c r="H57" s="1" t="s">
-        <v>114</v>
+        <v>120</v>
       </c>
       <c r="I57" s="1" t="b">
         <v>0</v>
       </c>
       <c r="J57" s="2" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
       <c r="K57" s="1" t="s">
         <v>16</v>
@@ -2825,22 +2977,31 @@
         <v>321004.0</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>113</v>
+        <v>119</v>
       </c>
       <c r="C58" s="1">
         <v>321.0</v>
       </c>
+      <c r="D58" s="1">
+        <v>141004.0</v>
+      </c>
       <c r="E58" s="1">
         <v>4.0</v>
       </c>
+      <c r="F58" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G58" s="1" t="b">
+        <v>1</v>
+      </c>
       <c r="H58" s="1" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
       <c r="I58" s="1" t="b">
         <v>0</v>
       </c>
       <c r="J58" s="2" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="K58" s="1" t="s">
         <v>16</v>
@@ -2851,22 +3012,31 @@
         <v>322004.0</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>113</v>
+        <v>119</v>
       </c>
       <c r="C59" s="1">
         <v>322.0</v>
       </c>
+      <c r="D59" s="1">
+        <v>141004.0</v>
+      </c>
       <c r="E59" s="1">
         <v>4.0</v>
       </c>
+      <c r="F59" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G59" s="1" t="b">
+        <v>1</v>
+      </c>
       <c r="H59" s="1" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="I59" s="1" t="b">
         <v>0</v>
       </c>
       <c r="J59" s="2" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="K59" s="1" t="s">
         <v>16</v>
@@ -2877,22 +3047,31 @@
         <v>323004.0</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>113</v>
+        <v>119</v>
       </c>
       <c r="C60" s="1">
         <v>323.0</v>
       </c>
+      <c r="D60" s="1">
+        <v>141004.0</v>
+      </c>
       <c r="E60" s="1">
         <v>4.0</v>
       </c>
+      <c r="F60" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G60" s="1" t="b">
+        <v>1</v>
+      </c>
       <c r="H60" s="1" t="s">
-        <v>120</v>
+        <v>126</v>
       </c>
       <c r="I60" s="1" t="b">
         <v>0</v>
       </c>
       <c r="J60" s="2" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
       <c r="K60" s="1" t="s">
         <v>16</v>
@@ -2903,22 +3082,31 @@
         <v>201005.0</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>122</v>
+        <v>128</v>
       </c>
       <c r="C61" s="1">
         <v>201.0</v>
       </c>
+      <c r="D61" s="1" t="b">
+        <v>0</v>
+      </c>
       <c r="E61" s="1">
         <v>4.0</v>
       </c>
+      <c r="F61" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G61" s="1" t="b">
+        <v>1</v>
+      </c>
       <c r="H61" s="1" t="s">
-        <v>123</v>
+        <v>129</v>
       </c>
       <c r="I61" s="1" t="b">
         <v>0</v>
       </c>
       <c r="J61" s="2" t="s">
-        <v>124</v>
+        <v>130</v>
       </c>
       <c r="K61" s="1" t="s">
         <v>16</v>
@@ -2929,22 +3117,31 @@
         <v>202005.0</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>122</v>
+        <v>128</v>
       </c>
       <c r="C62" s="1">
         <v>202.0</v>
       </c>
+      <c r="D62" s="1" t="b">
+        <v>0</v>
+      </c>
       <c r="E62" s="1">
         <v>4.0</v>
       </c>
+      <c r="F62" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G62" s="1" t="b">
+        <v>1</v>
+      </c>
       <c r="H62" s="1" t="s">
-        <v>125</v>
+        <v>131</v>
       </c>
       <c r="I62" s="1" t="b">
         <v>0</v>
       </c>
       <c r="J62" s="2" t="s">
-        <v>124</v>
+        <v>130</v>
       </c>
       <c r="K62" s="1" t="s">
         <v>16</v>
@@ -2955,22 +3152,31 @@
         <v>203005.0</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>122</v>
+        <v>128</v>
       </c>
       <c r="C63" s="1">
         <v>203.0</v>
       </c>
+      <c r="D63" s="1" t="b">
+        <v>0</v>
+      </c>
       <c r="E63" s="1">
         <v>4.0</v>
       </c>
+      <c r="F63" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G63" s="1" t="b">
+        <v>1</v>
+      </c>
       <c r="H63" s="1" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
       <c r="I63" s="1" t="b">
         <v>0</v>
       </c>
       <c r="J63" s="2" t="s">
-        <v>124</v>
+        <v>130</v>
       </c>
       <c r="K63" s="1" t="s">
         <v>16</v>
@@ -2981,22 +3187,31 @@
         <v>201006.0</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>127</v>
+        <v>133</v>
       </c>
       <c r="C64" s="1">
         <v>201.0</v>
       </c>
+      <c r="D64" s="1" t="b">
+        <v>0</v>
+      </c>
       <c r="E64" s="1">
         <v>4.0</v>
       </c>
+      <c r="F64" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="G64" s="1" t="b">
+        <v>1</v>
+      </c>
       <c r="H64" s="1" t="s">
-        <v>128</v>
+        <v>134</v>
       </c>
       <c r="I64" s="1" t="b">
         <v>0</v>
       </c>
       <c r="J64" s="2" t="s">
-        <v>129</v>
+        <v>135</v>
       </c>
       <c r="K64" s="1" t="s">
         <v>16</v>
@@ -3007,7 +3222,7 @@
         <v>348006.0</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>127</v>
+        <v>133</v>
       </c>
       <c r="C65" s="1">
         <v>348.0</v>
@@ -3015,17 +3230,26 @@
       <c r="E65" s="1">
         <v>4.0</v>
       </c>
+      <c r="F65" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G65" s="1" t="b">
+        <v>0</v>
+      </c>
       <c r="H65" s="1" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="I65" s="1" t="b">
         <v>0</v>
       </c>
       <c r="J65" s="2" t="s">
-        <v>131</v>
+        <v>137</v>
       </c>
       <c r="K65" s="1" t="s">
         <v>16</v>
+      </c>
+      <c r="L65" s="1" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="66">
@@ -3033,22 +3257,31 @@
         <v>301006.0</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>127</v>
+        <v>133</v>
       </c>
       <c r="C66" s="1">
         <v>301.0</v>
       </c>
+      <c r="D66" s="1" t="b">
+        <v>0</v>
+      </c>
       <c r="E66" s="1">
         <v>4.0</v>
       </c>
+      <c r="F66" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="G66" s="1" t="b">
+        <v>1</v>
+      </c>
       <c r="H66" s="1" t="s">
-        <v>132</v>
+        <v>139</v>
       </c>
       <c r="I66" s="1" t="b">
         <v>0</v>
       </c>
       <c r="J66" s="2" t="s">
-        <v>129</v>
+        <v>135</v>
       </c>
       <c r="K66" s="1" t="s">
         <v>16</v>
@@ -3059,22 +3292,31 @@
         <v>304006.0</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>127</v>
+        <v>133</v>
       </c>
       <c r="C67" s="1">
         <v>304.0</v>
       </c>
+      <c r="D67" s="1">
+        <v>201006.0</v>
+      </c>
       <c r="E67" s="1">
         <v>4.0</v>
       </c>
+      <c r="F67" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="G67" s="1" t="b">
+        <v>1</v>
+      </c>
       <c r="H67" s="1" t="s">
-        <v>133</v>
+        <v>140</v>
       </c>
       <c r="I67" s="1" t="b">
         <v>0</v>
       </c>
       <c r="J67" s="2" t="s">
-        <v>134</v>
+        <v>141</v>
       </c>
       <c r="K67" s="1" t="s">
         <v>16</v>
@@ -3085,22 +3327,31 @@
         <v>305006.0</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>127</v>
+        <v>133</v>
       </c>
       <c r="C68" s="1">
         <v>305.0</v>
       </c>
+      <c r="D68" s="1">
+        <v>201006.0</v>
+      </c>
       <c r="E68" s="1">
         <v>4.0</v>
       </c>
+      <c r="F68" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G68" s="1" t="b">
+        <v>1</v>
+      </c>
       <c r="H68" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="I68" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="J68" s="2" t="s">
         <v>135</v>
-      </c>
-      <c r="I68" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="J68" s="2" t="s">
-        <v>129</v>
       </c>
       <c r="K68" s="1" t="s">
         <v>16</v>
@@ -3111,22 +3362,31 @@
         <v>111003.0</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="C69" s="1">
         <v>111.0</v>
       </c>
+      <c r="D69" s="1">
+        <v>112001.0</v>
+      </c>
       <c r="E69" s="1">
         <v>4.0</v>
       </c>
+      <c r="F69" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G69" s="1" t="b">
+        <v>1</v>
+      </c>
       <c r="H69" s="1" t="s">
-        <v>136</v>
+        <v>143</v>
       </c>
       <c r="I69" s="1" t="b">
         <v>0</v>
       </c>
       <c r="J69" s="2" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="K69" s="1" t="s">
         <v>16</v>
@@ -3137,7 +3397,7 @@
         <v>113003.0</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="C70" s="1">
         <v>113.0</v>
@@ -3146,10 +3406,13 @@
         <v>4.0</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
+      </c>
+      <c r="G70" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="H70" s="1" t="s">
-        <v>137</v>
+        <v>144</v>
       </c>
       <c r="I70" s="1" t="b">
         <v>0</v>
@@ -3169,22 +3432,31 @@
         <v>211007.0</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>139</v>
+        <v>145</v>
       </c>
       <c r="C71" s="1">
         <v>211.0</v>
       </c>
+      <c r="D71" s="1">
+        <v>111003.0</v>
+      </c>
       <c r="E71" s="1">
         <v>4.0</v>
       </c>
+      <c r="F71" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G71" s="1" t="b">
+        <v>1</v>
+      </c>
       <c r="H71" s="1" t="s">
-        <v>140</v>
+        <v>146</v>
       </c>
       <c r="I71" s="1" t="b">
         <v>0</v>
       </c>
       <c r="J71" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="K71" s="1" t="s">
         <v>16</v>
@@ -3195,22 +3467,31 @@
         <v>212007.0</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>139</v>
+        <v>145</v>
       </c>
       <c r="C72" s="1">
         <v>212.0</v>
       </c>
+      <c r="D72" s="1">
+        <v>211007.0</v>
+      </c>
       <c r="E72" s="1">
         <v>4.0</v>
       </c>
+      <c r="F72" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G72" s="1" t="b">
+        <v>1</v>
+      </c>
       <c r="H72" s="1" t="s">
-        <v>141</v>
+        <v>147</v>
       </c>
       <c r="I72" s="1" t="b">
         <v>0</v>
       </c>
       <c r="J72" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="K72" s="1" t="s">
         <v>16</v>
@@ -3221,22 +3502,31 @@
         <v>213007.0</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>139</v>
+        <v>145</v>
       </c>
       <c r="C73" s="1">
         <v>213.0</v>
       </c>
+      <c r="D73" s="1">
+        <v>211007.0</v>
+      </c>
       <c r="E73" s="1">
         <v>4.0</v>
       </c>
+      <c r="F73" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G73" s="1" t="b">
+        <v>1</v>
+      </c>
       <c r="H73" s="1" t="s">
-        <v>142</v>
+        <v>148</v>
       </c>
       <c r="I73" s="1" t="b">
         <v>0</v>
       </c>
       <c r="J73" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="K73" s="1" t="s">
         <v>16</v>
@@ -3247,7 +3537,7 @@
         <v>121008.0</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>143</v>
+        <v>149</v>
       </c>
       <c r="C74" s="1">
         <v>121.0</v>
@@ -3258,11 +3548,14 @@
       <c r="E74" s="1">
         <v>4.0</v>
       </c>
+      <c r="F74" s="1" t="s">
+        <v>51</v>
+      </c>
       <c r="G74" s="1" t="b">
         <v>1</v>
       </c>
       <c r="H74" s="1" t="s">
-        <v>144</v>
+        <v>150</v>
       </c>
       <c r="I74" s="1" t="b">
         <v>1</v>
@@ -3279,7 +3572,7 @@
         <v>122008.0</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>143</v>
+        <v>149</v>
       </c>
       <c r="C75" s="1">
         <v>122.0</v>
@@ -3290,11 +3583,14 @@
       <c r="E75" s="1">
         <v>4.0</v>
       </c>
+      <c r="F75" s="1" t="s">
+        <v>51</v>
+      </c>
       <c r="G75" s="1" t="b">
         <v>1</v>
       </c>
       <c r="H75" s="1" t="s">
-        <v>144</v>
+        <v>150</v>
       </c>
       <c r="I75" s="1" t="b">
         <v>1</v>
@@ -3311,7 +3607,7 @@
         <v>320008.0</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>143</v>
+        <v>149</v>
       </c>
       <c r="C76" s="1">
         <v>320.0</v>
@@ -3322,11 +3618,14 @@
       <c r="E76" s="1">
         <v>4.0</v>
       </c>
+      <c r="F76" s="1" t="s">
+        <v>51</v>
+      </c>
       <c r="G76" s="1" t="b">
         <v>1</v>
       </c>
       <c r="H76" s="1" t="s">
-        <v>145</v>
+        <v>151</v>
       </c>
       <c r="I76" s="1" t="b">
         <v>0</v>
@@ -3336,6 +3635,9 @@
       </c>
       <c r="K76" s="1" t="s">
         <v>16</v>
+      </c>
+      <c r="L76" s="1" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="77">
@@ -3343,7 +3645,7 @@
         <v>321008.0</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>143</v>
+        <v>149</v>
       </c>
       <c r="C77" s="1">
         <v>321.0</v>
@@ -3354,20 +3656,26 @@
       <c r="E77" s="1">
         <v>4.0</v>
       </c>
+      <c r="F77" s="1" t="s">
+        <v>51</v>
+      </c>
       <c r="G77" s="1" t="b">
         <v>1</v>
       </c>
       <c r="H77" s="1" t="s">
-        <v>146</v>
+        <v>153</v>
       </c>
       <c r="I77" s="1" t="b">
         <v>0</v>
       </c>
       <c r="J77" s="2" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
       <c r="K77" s="1" t="s">
         <v>16</v>
+      </c>
+      <c r="L77" s="1" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="78">
@@ -3375,7 +3683,7 @@
         <v>253001.0</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C78" s="1">
         <v>253.0</v>
@@ -3386,20 +3694,23 @@
       <c r="E78" s="1">
         <v>4.0</v>
       </c>
+      <c r="F78" s="1" t="s">
+        <v>51</v>
+      </c>
       <c r="G78" s="1" t="b">
         <v>1</v>
       </c>
       <c r="H78" s="1" t="s">
-        <v>148</v>
+        <v>155</v>
       </c>
       <c r="I78" s="1" t="b">
         <v>0</v>
       </c>
       <c r="J78" s="2" t="s">
-        <v>149</v>
+        <v>156</v>
       </c>
       <c r="K78" s="1" t="s">
-        <v>150</v>
+        <v>157</v>
       </c>
     </row>
     <row r="79">
@@ -3407,7 +3718,7 @@
         <v>281001.0</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C79" s="1">
         <v>281.0</v>
@@ -3418,17 +3729,23 @@
       <c r="E79" s="1">
         <v>4.0</v>
       </c>
+      <c r="F79" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G79" s="1" t="b">
+        <v>1</v>
+      </c>
       <c r="H79" s="1" t="s">
-        <v>151</v>
+        <v>158</v>
       </c>
       <c r="I79" s="1" t="b">
         <v>0</v>
       </c>
       <c r="J79" s="2" t="s">
-        <v>149</v>
+        <v>156</v>
       </c>
       <c r="K79" s="1" t="s">
-        <v>150</v>
+        <v>157</v>
       </c>
     </row>
     <row r="80">
@@ -3436,7 +3753,7 @@
         <v>256001.0</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C80" s="1">
         <v>256.0</v>
@@ -3447,17 +3764,23 @@
       <c r="E80" s="1">
         <v>4.0</v>
       </c>
+      <c r="F80" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="G80" s="1" t="b">
+        <v>1</v>
+      </c>
       <c r="H80" s="1" t="s">
-        <v>152</v>
+        <v>159</v>
       </c>
       <c r="I80" s="1" t="b">
         <v>0</v>
       </c>
       <c r="J80" s="2" t="s">
-        <v>149</v>
+        <v>156</v>
       </c>
       <c r="K80" s="1" t="s">
-        <v>150</v>
+        <v>157</v>
       </c>
     </row>
     <row r="81">
@@ -3465,7 +3788,7 @@
         <v>282001.0</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C81" s="1">
         <v>282.0</v>
@@ -3476,17 +3799,23 @@
       <c r="E81" s="1">
         <v>4.0</v>
       </c>
+      <c r="F81" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G81" s="1" t="b">
+        <v>1</v>
+      </c>
       <c r="H81" s="1" t="s">
-        <v>153</v>
+        <v>160</v>
       </c>
       <c r="I81" s="1" t="b">
         <v>0</v>
       </c>
       <c r="J81" s="2" t="s">
-        <v>149</v>
+        <v>156</v>
       </c>
       <c r="K81" s="1" t="s">
-        <v>150</v>
+        <v>157</v>
       </c>
     </row>
     <row r="82">
@@ -3494,7 +3823,7 @@
         <v>307001.0</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C82" s="1">
         <v>307.0</v>
@@ -3505,17 +3834,26 @@
       <c r="E82" s="1">
         <v>4.0</v>
       </c>
+      <c r="F82" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="G82" s="1" t="b">
+        <v>1</v>
+      </c>
       <c r="H82" s="1" t="s">
-        <v>154</v>
+        <v>161</v>
       </c>
       <c r="I82" s="1" t="b">
         <v>0</v>
       </c>
       <c r="J82" s="2" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="K82" s="1" t="s">
-        <v>150</v>
+        <v>157</v>
+      </c>
+      <c r="L82" s="1" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="83">
@@ -3523,25 +3861,34 @@
         <v>316001.0</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C83" s="1">
         <v>316.0</v>
       </c>
+      <c r="D83" s="1" t="s">
+        <v>164</v>
+      </c>
       <c r="E83" s="1">
         <v>4.0</v>
       </c>
+      <c r="F83" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="G83" s="1" t="b">
+        <v>1</v>
+      </c>
       <c r="H83" s="1" t="s">
-        <v>156</v>
+        <v>165</v>
       </c>
       <c r="I83" s="1" t="b">
         <v>0</v>
       </c>
       <c r="J83" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="K83" s="1" t="s">
-        <v>150</v>
+        <v>157</v>
       </c>
     </row>
     <row r="84">
@@ -3549,7 +3896,7 @@
         <v>317001.0</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C84" s="1">
         <v>317.0</v>
@@ -3560,17 +3907,23 @@
       <c r="E84" s="1">
         <v>4.0</v>
       </c>
+      <c r="F84" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G84" s="1" t="b">
+        <v>1</v>
+      </c>
       <c r="H84" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="I84" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="J84" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="K84" s="1" t="s">
         <v>157</v>
-      </c>
-      <c r="I84" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="J84" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="K84" s="1" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="85">
@@ -3578,25 +3931,37 @@
         <v>320001.0</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C85" s="1">
         <v>320.0</v>
       </c>
+      <c r="D85" s="1" t="s">
+        <v>167</v>
+      </c>
       <c r="E85" s="1">
         <v>4.0</v>
       </c>
+      <c r="F85" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G85" s="1" t="b">
+        <v>0</v>
+      </c>
       <c r="H85" s="1" t="s">
-        <v>158</v>
+        <v>168</v>
       </c>
       <c r="I85" s="1" t="b">
         <v>0</v>
       </c>
       <c r="J85" s="2" t="s">
-        <v>149</v>
+        <v>156</v>
       </c>
       <c r="K85" s="1" t="s">
-        <v>150</v>
+        <v>157</v>
+      </c>
+      <c r="L85" s="1" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="86">
@@ -3604,25 +3969,34 @@
         <v>345001.0</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C86" s="1">
         <v>345.0</v>
       </c>
+      <c r="D86" s="1" t="s">
+        <v>170</v>
+      </c>
       <c r="E86" s="1">
         <v>4.0</v>
       </c>
+      <c r="F86" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G86" s="1" t="b">
+        <v>1</v>
+      </c>
       <c r="H86" s="1" t="s">
-        <v>159</v>
+        <v>171</v>
       </c>
       <c r="I86" s="1" t="b">
         <v>0</v>
       </c>
       <c r="J86" s="2" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="K86" s="1" t="s">
-        <v>150</v>
+        <v>157</v>
       </c>
     </row>
     <row r="87">
@@ -3630,25 +4004,34 @@
         <v>347001.0</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C87" s="1">
         <v>347.0</v>
       </c>
+      <c r="D87" s="1" t="s">
+        <v>164</v>
+      </c>
       <c r="E87" s="1">
         <v>4.0</v>
       </c>
+      <c r="F87" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G87" s="1" t="b">
+        <v>1</v>
+      </c>
       <c r="H87" s="1" t="s">
-        <v>160</v>
+        <v>172</v>
       </c>
       <c r="I87" s="1" t="b">
         <v>0</v>
       </c>
       <c r="J87" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="K87" s="1" t="s">
-        <v>150</v>
+        <v>157</v>
       </c>
     </row>
     <row r="88">
@@ -3656,7 +4039,7 @@
         <v>348001.0</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C88" s="1">
         <v>348.0</v>
@@ -3667,17 +4050,23 @@
       <c r="E88" s="1">
         <v>4.0</v>
       </c>
+      <c r="F88" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G88" s="1" t="b">
+        <v>1</v>
+      </c>
       <c r="H88" s="1" t="s">
-        <v>161</v>
+        <v>173</v>
       </c>
       <c r="I88" s="1" t="b">
         <v>0</v>
       </c>
       <c r="J88" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="K88" s="1" t="s">
-        <v>150</v>
+        <v>157</v>
       </c>
     </row>
     <row r="89">
@@ -3685,25 +4074,34 @@
         <v>351001.0</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C89" s="1">
         <v>351.0</v>
       </c>
+      <c r="D89" s="1" t="s">
+        <v>164</v>
+      </c>
       <c r="E89" s="1">
         <v>4.0</v>
       </c>
+      <c r="F89" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G89" s="1" t="b">
+        <v>1</v>
+      </c>
       <c r="H89" s="1" t="s">
-        <v>162</v>
+        <v>174</v>
       </c>
       <c r="I89" s="1" t="b">
         <v>0</v>
       </c>
       <c r="J89" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="K89" s="1" t="s">
-        <v>150</v>
+        <v>157</v>
       </c>
     </row>
     <row r="90">
@@ -3711,7 +4109,7 @@
         <v>352001.0</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C90" s="1">
         <v>352.0</v>
@@ -3722,17 +4120,23 @@
       <c r="E90" s="1">
         <v>4.0</v>
       </c>
+      <c r="F90" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G90" s="1" t="b">
+        <v>1</v>
+      </c>
       <c r="H90" s="1" t="s">
-        <v>163</v>
+        <v>175</v>
       </c>
       <c r="I90" s="1" t="b">
         <v>0</v>
       </c>
       <c r="J90" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="K90" s="1" t="s">
-        <v>150</v>
+        <v>157</v>
       </c>
     </row>
     <row r="91">
@@ -3740,25 +4144,34 @@
         <v>391001.0</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C91" s="1">
         <v>391.0</v>
       </c>
+      <c r="D91" s="1" t="s">
+        <v>176</v>
+      </c>
       <c r="E91" s="1">
         <v>4.0</v>
       </c>
+      <c r="F91" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G91" s="1" t="b">
+        <v>1</v>
+      </c>
       <c r="H91" s="1" t="s">
-        <v>164</v>
+        <v>177</v>
       </c>
       <c r="I91" s="1" t="b">
         <v>0</v>
       </c>
       <c r="J91" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="K91" s="1" t="s">
-        <v>150</v>
+        <v>157</v>
       </c>
     </row>
     <row r="92">
@@ -3766,7 +4179,7 @@
         <v>392001.0</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C92" s="1">
         <v>392.0</v>
@@ -3777,17 +4190,23 @@
       <c r="E92" s="1">
         <v>4.0</v>
       </c>
+      <c r="F92" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G92" s="1" t="b">
+        <v>1</v>
+      </c>
       <c r="H92" s="1" t="s">
-        <v>165</v>
+        <v>178</v>
       </c>
       <c r="I92" s="1" t="b">
         <v>0</v>
       </c>
       <c r="J92" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="K92" s="1" t="s">
-        <v>150</v>
+        <v>157</v>
       </c>
     </row>
     <row r="93">
@@ -3795,25 +4214,34 @@
         <v>394001.0</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C93" s="1">
         <v>394.0</v>
       </c>
+      <c r="D93" s="1" t="s">
+        <v>164</v>
+      </c>
       <c r="E93" s="1">
         <v>4.0</v>
       </c>
+      <c r="F93" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G93" s="1" t="b">
+        <v>1</v>
+      </c>
       <c r="H93" s="1" t="s">
-        <v>166</v>
+        <v>179</v>
       </c>
       <c r="I93" s="1" t="b">
         <v>0</v>
       </c>
       <c r="J93" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="K93" s="1" t="s">
-        <v>150</v>
+        <v>157</v>
       </c>
     </row>
     <row r="94">
@@ -3821,7 +4249,7 @@
         <v>395001.0</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C94" s="1">
         <v>395.0</v>
@@ -3832,17 +4260,23 @@
       <c r="E94" s="1">
         <v>4.0</v>
       </c>
+      <c r="F94" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G94" s="1" t="b">
+        <v>1</v>
+      </c>
       <c r="H94" s="1" t="s">
-        <v>167</v>
+        <v>180</v>
       </c>
       <c r="I94" s="1" t="b">
         <v>0</v>
       </c>
       <c r="J94" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="K94" s="1" t="s">
-        <v>150</v>
+        <v>157</v>
       </c>
     </row>
     <row r="95">
@@ -3850,25 +4284,34 @@
         <v>397001.0</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C95" s="1">
         <v>397.0</v>
       </c>
+      <c r="D95" s="1" t="s">
+        <v>164</v>
+      </c>
       <c r="E95" s="1">
         <v>4.0</v>
       </c>
+      <c r="F95" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G95" s="1" t="b">
+        <v>1</v>
+      </c>
       <c r="H95" s="1" t="s">
-        <v>168</v>
+        <v>181</v>
       </c>
       <c r="I95" s="1" t="b">
         <v>0</v>
       </c>
       <c r="J95" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="K95" s="1" t="s">
-        <v>150</v>
+        <v>157</v>
       </c>
     </row>
     <row r="96">
@@ -3876,25 +4319,34 @@
         <v>411001.0</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C96" s="1">
         <v>411.0</v>
       </c>
+      <c r="D96" s="1" t="s">
+        <v>182</v>
+      </c>
       <c r="E96" s="1">
         <v>4.0</v>
       </c>
+      <c r="F96" s="1" t="s">
+        <v>39</v>
+      </c>
       <c r="H96" s="1" t="s">
-        <v>169</v>
+        <v>183</v>
       </c>
       <c r="I96" s="1" t="b">
         <v>0</v>
       </c>
       <c r="J96" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="K96" s="1" t="s">
-        <v>150</v>
+        <v>157</v>
+      </c>
+      <c r="L96" s="1" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="97">
@@ -3902,7 +4354,7 @@
         <v>412001.0</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C97" s="1">
         <v>412.0</v>
@@ -3910,17 +4362,23 @@
       <c r="E97" s="1">
         <v>4.0</v>
       </c>
+      <c r="F97" s="1" t="s">
+        <v>39</v>
+      </c>
       <c r="H97" s="1" t="s">
-        <v>170</v>
+        <v>184</v>
       </c>
       <c r="I97" s="1" t="b">
         <v>0</v>
       </c>
       <c r="J97" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="K97" s="1" t="s">
-        <v>150</v>
+        <v>157</v>
+      </c>
+      <c r="L97" s="1" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="98">
@@ -3928,7 +4386,7 @@
         <v>413001.0</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C98" s="1">
         <v>413.0</v>
@@ -3936,17 +4394,23 @@
       <c r="E98" s="1">
         <v>4.0</v>
       </c>
+      <c r="F98" s="1" t="s">
+        <v>39</v>
+      </c>
       <c r="H98" s="1" t="s">
-        <v>171</v>
+        <v>185</v>
       </c>
       <c r="I98" s="1" t="b">
         <v>0</v>
       </c>
       <c r="J98" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="K98" s="1" t="s">
-        <v>150</v>
+        <v>157</v>
+      </c>
+      <c r="L98" s="1" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="99">
@@ -3954,25 +4418,34 @@
         <v>414001.0</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C99" s="1">
         <v>414.0</v>
       </c>
+      <c r="D99" s="1">
+        <v>413001.0</v>
+      </c>
       <c r="E99" s="1">
         <v>4.0</v>
       </c>
+      <c r="F99" s="1" t="s">
+        <v>39</v>
+      </c>
       <c r="H99" s="1" t="s">
-        <v>172</v>
+        <v>186</v>
       </c>
       <c r="I99" s="1" t="b">
         <v>0</v>
       </c>
       <c r="J99" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="K99" s="1" t="s">
-        <v>150</v>
+        <v>157</v>
+      </c>
+      <c r="L99" s="1" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="100">
@@ -3980,7 +4453,7 @@
         <v>415001.0</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C100" s="1">
         <v>415.0</v>
@@ -3988,17 +4461,23 @@
       <c r="E100" s="1">
         <v>4.0</v>
       </c>
+      <c r="F100" s="1" t="s">
+        <v>39</v>
+      </c>
       <c r="H100" s="1" t="s">
-        <v>173</v>
+        <v>187</v>
       </c>
       <c r="I100" s="1" t="b">
         <v>0</v>
       </c>
       <c r="J100" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="K100" s="1" t="s">
-        <v>150</v>
+        <v>157</v>
+      </c>
+      <c r="L100" s="1" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="101">
@@ -4006,7 +4485,7 @@
         <v>421001.0</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C101" s="1">
         <v>421.0</v>
@@ -4014,17 +4493,23 @@
       <c r="E101" s="1">
         <v>4.0</v>
       </c>
+      <c r="F101" s="1" t="s">
+        <v>39</v>
+      </c>
       <c r="H101" s="1" t="s">
-        <v>174</v>
+        <v>188</v>
       </c>
       <c r="I101" s="1" t="b">
         <v>0</v>
       </c>
       <c r="J101" s="2" t="s">
-        <v>149</v>
+        <v>156</v>
       </c>
       <c r="K101" s="1" t="s">
-        <v>150</v>
+        <v>157</v>
+      </c>
+      <c r="L101" s="1" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="102">
@@ -4032,7 +4517,7 @@
         <v>422001.0</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C102" s="1">
         <v>422.0</v>
@@ -4040,17 +4525,23 @@
       <c r="E102" s="1">
         <v>4.0</v>
       </c>
+      <c r="F102" s="1" t="s">
+        <v>39</v>
+      </c>
       <c r="H102" s="1" t="s">
-        <v>175</v>
+        <v>189</v>
       </c>
       <c r="I102" s="1" t="b">
         <v>0</v>
       </c>
       <c r="J102" s="2" t="s">
-        <v>149</v>
+        <v>156</v>
       </c>
       <c r="K102" s="1" t="s">
-        <v>150</v>
+        <v>157</v>
+      </c>
+      <c r="L102" s="1" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="103">
@@ -4058,7 +4549,7 @@
         <v>431001.0</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C103" s="1">
         <v>431.0</v>
@@ -4066,17 +4557,23 @@
       <c r="E103" s="1">
         <v>4.0</v>
       </c>
+      <c r="F103" s="1" t="s">
+        <v>39</v>
+      </c>
       <c r="H103" s="1" t="s">
-        <v>176</v>
+        <v>190</v>
       </c>
       <c r="I103" s="1" t="b">
         <v>0</v>
       </c>
       <c r="J103" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="K103" s="1" t="s">
-        <v>150</v>
+        <v>157</v>
+      </c>
+      <c r="L103" s="1" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="104">
@@ -4084,7 +4581,7 @@
         <v>432001.0</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C104" s="1">
         <v>432.0</v>
@@ -4092,17 +4589,23 @@
       <c r="E104" s="1">
         <v>4.0</v>
       </c>
+      <c r="F104" s="1" t="s">
+        <v>39</v>
+      </c>
       <c r="H104" s="1" t="s">
-        <v>177</v>
+        <v>191</v>
       </c>
       <c r="I104" s="1" t="b">
         <v>0</v>
       </c>
       <c r="J104" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="K104" s="1" t="s">
-        <v>150</v>
+        <v>157</v>
+      </c>
+      <c r="L104" s="1" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="105">
@@ -4110,7 +4613,7 @@
         <v>433001.0</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C105" s="1">
         <v>433.0</v>
@@ -4118,17 +4621,23 @@
       <c r="E105" s="1">
         <v>4.0</v>
       </c>
+      <c r="F105" s="1" t="s">
+        <v>39</v>
+      </c>
       <c r="H105" s="1" t="s">
-        <v>178</v>
+        <v>192</v>
       </c>
       <c r="I105" s="1" t="b">
         <v>0</v>
       </c>
       <c r="J105" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="K105" s="1" t="s">
-        <v>150</v>
+        <v>157</v>
+      </c>
+      <c r="L105" s="1" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="106">
@@ -4136,7 +4645,7 @@
         <v>434001.0</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C106" s="1">
         <v>434.0</v>
@@ -4144,17 +4653,23 @@
       <c r="E106" s="1">
         <v>4.0</v>
       </c>
+      <c r="F106" s="1" t="s">
+        <v>39</v>
+      </c>
       <c r="H106" s="1" t="s">
-        <v>179</v>
+        <v>193</v>
       </c>
       <c r="I106" s="1" t="b">
         <v>0</v>
       </c>
       <c r="J106" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="K106" s="1" t="s">
-        <v>150</v>
+        <v>157</v>
+      </c>
+      <c r="L106" s="1" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="107">
@@ -4162,7 +4677,7 @@
         <v>441001.0</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C107" s="1">
         <v>441.0</v>
@@ -4170,17 +4685,23 @@
       <c r="E107" s="1">
         <v>4.0</v>
       </c>
+      <c r="F107" s="1" t="s">
+        <v>39</v>
+      </c>
       <c r="H107" s="1" t="s">
-        <v>180</v>
+        <v>194</v>
       </c>
       <c r="I107" s="1" t="b">
         <v>0</v>
       </c>
       <c r="J107" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="K107" s="1" t="s">
-        <v>150</v>
+        <v>157</v>
+      </c>
+      <c r="L107" s="1" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="108">
@@ -4188,7 +4709,7 @@
         <v>444001.0</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C108" s="1">
         <v>444.0</v>
@@ -4196,17 +4717,23 @@
       <c r="E108" s="1">
         <v>4.0</v>
       </c>
+      <c r="F108" s="1" t="s">
+        <v>39</v>
+      </c>
       <c r="H108" s="1" t="s">
-        <v>181</v>
+        <v>195</v>
       </c>
       <c r="I108" s="1" t="b">
         <v>0</v>
       </c>
       <c r="J108" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="K108" s="1" t="s">
-        <v>150</v>
+        <v>157</v>
+      </c>
+      <c r="L108" s="1" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="109">
@@ -4214,7 +4741,7 @@
         <v>445001.0</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C109" s="1">
         <v>445.0</v>
@@ -4222,17 +4749,23 @@
       <c r="E109" s="1">
         <v>4.0</v>
       </c>
+      <c r="F109" s="1" t="s">
+        <v>39</v>
+      </c>
       <c r="H109" s="1" t="s">
-        <v>182</v>
+        <v>196</v>
       </c>
       <c r="I109" s="1" t="b">
         <v>0</v>
       </c>
       <c r="J109" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="K109" s="1" t="s">
-        <v>150</v>
+        <v>157</v>
+      </c>
+      <c r="L109" s="1" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="110">
@@ -4240,7 +4773,7 @@
         <v>446001.0</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C110" s="1">
         <v>446.0</v>
@@ -4248,17 +4781,23 @@
       <c r="E110" s="1">
         <v>4.0</v>
       </c>
+      <c r="F110" s="1" t="s">
+        <v>39</v>
+      </c>
       <c r="H110" s="1" t="s">
-        <v>183</v>
+        <v>197</v>
       </c>
       <c r="I110" s="1" t="b">
         <v>0</v>
       </c>
       <c r="J110" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="K110" s="1" t="s">
-        <v>150</v>
+        <v>157</v>
+      </c>
+      <c r="L110" s="1" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="111">
@@ -4266,7 +4805,7 @@
         <v>461001.0</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C111" s="1">
         <v>461.0</v>
@@ -4274,17 +4813,23 @@
       <c r="E111" s="1">
         <v>4.0</v>
       </c>
+      <c r="F111" s="1" t="s">
+        <v>39</v>
+      </c>
       <c r="H111" s="1" t="s">
-        <v>184</v>
+        <v>198</v>
       </c>
       <c r="I111" s="1" t="b">
         <v>0</v>
       </c>
       <c r="J111" s="2" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="K111" s="1" t="s">
-        <v>150</v>
+        <v>157</v>
+      </c>
+      <c r="L111" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="112">
@@ -4292,7 +4837,7 @@
         <v>462001.0</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C112" s="1">
         <v>462.0</v>
@@ -4300,17 +4845,23 @@
       <c r="E112" s="1">
         <v>4.0</v>
       </c>
+      <c r="F112" s="1" t="s">
+        <v>39</v>
+      </c>
       <c r="H112" s="1" t="s">
-        <v>185</v>
+        <v>199</v>
       </c>
       <c r="I112" s="1" t="b">
         <v>0</v>
       </c>
       <c r="J112" s="2" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="K112" s="1" t="s">
-        <v>150</v>
+        <v>157</v>
+      </c>
+      <c r="L112" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="113">
@@ -4318,7 +4869,7 @@
         <v>463001.0</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C113" s="1">
         <v>463.0</v>
@@ -4326,17 +4877,23 @@
       <c r="E113" s="1">
         <v>4.0</v>
       </c>
+      <c r="F113" s="1" t="s">
+        <v>39</v>
+      </c>
       <c r="H113" s="1" t="s">
-        <v>186</v>
+        <v>200</v>
       </c>
       <c r="I113" s="1" t="b">
         <v>0</v>
       </c>
       <c r="J113" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="K113" s="1" t="s">
-        <v>150</v>
+        <v>157</v>
+      </c>
+      <c r="L113" s="1" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="114">
@@ -4344,7 +4901,7 @@
         <v>467001.0</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C114" s="1">
         <v>467.0</v>
@@ -4352,17 +4909,129 @@
       <c r="E114" s="1">
         <v>4.0</v>
       </c>
+      <c r="F114" s="1" t="s">
+        <v>39</v>
+      </c>
       <c r="H114" s="1" t="s">
-        <v>187</v>
+        <v>201</v>
       </c>
       <c r="I114" s="1" t="b">
         <v>0</v>
       </c>
       <c r="J114" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="K114" s="1" t="s">
-        <v>150</v>
+        <v>157</v>
+      </c>
+      <c r="L114" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" s="1">
+        <v>425001.0</v>
+      </c>
+      <c r="B115" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C115" s="1">
+        <v>425.0</v>
+      </c>
+      <c r="D115" s="1">
+        <v>111001.0</v>
+      </c>
+      <c r="E115" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="F115" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="G115" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="H115" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="I115" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="J115" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="K115" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="L115" s="1"/>
+    </row>
+    <row r="116">
+      <c r="A116" s="1">
+        <v>111001.0</v>
+      </c>
+      <c r="B116" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C116" s="1">
+        <v>111.0</v>
+      </c>
+      <c r="D116" s="1">
+        <v>101001.0</v>
+      </c>
+      <c r="E116" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="F116" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="G116" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="H116" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="I116" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="J116" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="K116" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" s="1">
+        <v>101001.0</v>
+      </c>
+      <c r="B117" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C117" s="1">
+        <v>101.0</v>
+      </c>
+      <c r="D117" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E117" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="F117" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="G117" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="H117" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="I117" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="J117" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="K117" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add generic courses for gen ed credits
</commit_message>
<xml_diff>
--- a/cs_degree_planner/forecast/recommendcourses.xlsx
+++ b/cs_degree_planner/forecast/recommendcourses.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adam Case\Documents\School\cis422\cs422-proj2\cs422-proj2\cs_degree_planner\forecast\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zane\Documents\CS_folders\CS_422_p2\cs_degree_planner\forecast\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69D2B0D4-1FEC-4468-A6DD-837EDE96D83B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34767E8D-E86D-4755-A2EF-2E0E750EB1B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -159,7 +159,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="641" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="671" uniqueCount="230">
   <si>
     <t>id</t>
   </si>
@@ -813,6 +813,42 @@
   </si>
   <si>
     <t>Modeling</t>
+  </si>
+  <si>
+    <t>AAL</t>
+  </si>
+  <si>
+    <t>Generic Arts and Letters Credit</t>
+  </si>
+  <si>
+    <t>GP</t>
+  </si>
+  <si>
+    <t>SCI</t>
+  </si>
+  <si>
+    <t>SO</t>
+  </si>
+  <si>
+    <t>US</t>
+  </si>
+  <si>
+    <t>Generic US differences and inequalities Credit</t>
+  </si>
+  <si>
+    <t>Generic Global Perspectives Credit</t>
+  </si>
+  <si>
+    <t>Generic Science Credit</t>
+  </si>
+  <si>
+    <t>Generic Social Science Credit</t>
+  </si>
+  <si>
+    <t>CRE</t>
+  </si>
+  <si>
+    <t>Generic Credit (any)</t>
   </si>
 </sst>
 </file>
@@ -894,6 +930,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1097,10 +1137,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:L117"/>
+  <dimension ref="A1:L123"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView tabSelected="1" topLeftCell="A71" workbookViewId="0">
+      <selection activeCell="P84" sqref="P84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1109,7 +1149,7 @@
     <col min="10" max="10" width="37" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1147,7 +1187,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>210000</v>
       </c>
@@ -1185,7 +1225,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>211000</v>
       </c>
@@ -1220,7 +1260,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>212000</v>
       </c>
@@ -1255,7 +1295,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>313000</v>
       </c>
@@ -1290,7 +1330,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>314000</v>
       </c>
@@ -1325,7 +1365,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>315000</v>
       </c>
@@ -1360,7 +1400,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>333000</v>
       </c>
@@ -1395,7 +1435,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>322000</v>
       </c>
@@ -1430,7 +1470,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>443000</v>
       </c>
@@ -1465,7 +1505,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>451000</v>
       </c>
@@ -1500,7 +1540,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>453000</v>
       </c>
@@ -1535,7 +1575,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>4100001</v>
       </c>
@@ -1570,7 +1610,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>4100002</v>
       </c>
@@ -1605,7 +1645,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>4100003</v>
       </c>
@@ -1640,7 +1680,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>330000</v>
       </c>
@@ -1675,7 +1715,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>422000</v>
       </c>
@@ -1710,7 +1750,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>441000</v>
       </c>
@@ -1745,7 +1785,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>436000</v>
       </c>
@@ -1780,7 +1820,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>432000</v>
       </c>
@@ -1815,7 +1855,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>431000</v>
       </c>
@@ -1850,7 +1890,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>429000</v>
       </c>
@@ -1885,7 +1925,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>445000</v>
       </c>
@@ -1920,7 +1960,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>415000</v>
       </c>
@@ -1955,7 +1995,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>471000</v>
       </c>
@@ -1990,7 +2030,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>472000</v>
       </c>
@@ -2025,7 +2065,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>425000</v>
       </c>
@@ -2060,7 +2100,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>413000</v>
       </c>
@@ -2095,7 +2135,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>420000</v>
       </c>
@@ -2130,7 +2170,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>427000</v>
       </c>
@@ -2164,7 +2204,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>473000</v>
       </c>
@@ -2199,7 +2239,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>423000</v>
       </c>
@@ -2234,7 +2274,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>461000</v>
       </c>
@@ -2269,7 +2309,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
         <v>433000</v>
       </c>
@@ -2304,7 +2344,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
         <v>434000</v>
       </c>
@@ -2339,7 +2379,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
         <v>112001</v>
       </c>
@@ -2374,7 +2414,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
         <v>231001</v>
       </c>
@@ -2409,7 +2449,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
         <v>232001</v>
       </c>
@@ -2444,7 +2484,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
         <v>251001</v>
       </c>
@@ -2482,7 +2522,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
         <v>252001</v>
       </c>
@@ -2517,7 +2557,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
         <v>343001</v>
       </c>
@@ -2552,7 +2592,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
         <v>341001</v>
       </c>
@@ -2587,7 +2627,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
         <v>342001</v>
       </c>
@@ -2622,7 +2662,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
         <v>246001</v>
       </c>
@@ -2657,7 +2697,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
         <v>247001</v>
       </c>
@@ -2692,7 +2732,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
         <v>261001</v>
       </c>
@@ -2727,7 +2767,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
         <v>262001</v>
       </c>
@@ -2759,7 +2799,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
         <v>201002</v>
       </c>
@@ -2794,7 +2834,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
         <v>202002</v>
       </c>
@@ -2829,7 +2869,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
         <v>203002</v>
       </c>
@@ -2864,7 +2904,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
         <v>251002</v>
       </c>
@@ -2899,7 +2939,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
         <v>252002</v>
       </c>
@@ -2934,7 +2974,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
         <v>253002</v>
       </c>
@@ -2969,7 +3009,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A54" s="1">
         <v>221003</v>
       </c>
@@ -3004,7 +3044,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A55" s="1">
         <v>222003</v>
       </c>
@@ -3039,7 +3079,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A56" s="1">
         <v>223003</v>
       </c>
@@ -3074,7 +3114,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A57" s="1">
         <v>141004</v>
       </c>
@@ -3109,7 +3149,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A58" s="1">
         <v>321004</v>
       </c>
@@ -3144,7 +3184,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A59" s="1">
         <v>322004</v>
       </c>
@@ -3179,7 +3219,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A60" s="1">
         <v>323004</v>
       </c>
@@ -3214,7 +3254,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A61" s="1">
         <v>201005</v>
       </c>
@@ -3249,7 +3289,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A62" s="1">
         <v>202005</v>
       </c>
@@ -3284,7 +3324,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A63" s="1">
         <v>203005</v>
       </c>
@@ -3319,7 +3359,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A64" s="1">
         <v>201006</v>
       </c>
@@ -3354,7 +3394,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A65" s="1">
         <v>348006</v>
       </c>
@@ -3389,7 +3429,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A66" s="1">
         <v>301006</v>
       </c>
@@ -3424,7 +3464,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A67" s="1">
         <v>304006</v>
       </c>
@@ -3459,7 +3499,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A68" s="1">
         <v>305006</v>
       </c>
@@ -3494,7 +3534,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A69" s="1">
         <v>111003</v>
       </c>
@@ -3529,7 +3569,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A70" s="1">
         <v>113003</v>
       </c>
@@ -3564,7 +3604,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A71" s="1">
         <v>211007</v>
       </c>
@@ -3599,7 +3639,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A72" s="1">
         <v>212007</v>
       </c>
@@ -3634,7 +3674,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A73" s="1">
         <v>213007</v>
       </c>
@@ -3669,7 +3709,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A74" s="1">
         <v>121008</v>
       </c>
@@ -3704,7 +3744,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A75" s="1">
         <v>122008</v>
       </c>
@@ -3739,7 +3779,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A76" s="1">
         <v>320008</v>
       </c>
@@ -3777,7 +3817,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A77" s="1">
         <v>321008</v>
       </c>
@@ -3815,7 +3855,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A78" s="1">
         <v>253001</v>
       </c>
@@ -3850,7 +3890,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A79" s="1">
         <v>281001</v>
       </c>
@@ -3885,7 +3925,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A80" s="1">
         <v>256001</v>
       </c>
@@ -3920,7 +3960,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A81" s="1">
         <v>282001</v>
       </c>
@@ -3955,7 +3995,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A82" s="1">
         <v>307001</v>
       </c>
@@ -3993,7 +4033,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A83" s="1">
         <v>316001</v>
       </c>
@@ -4028,7 +4068,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A84" s="1">
         <v>317001</v>
       </c>
@@ -4063,7 +4103,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A85" s="1">
         <v>320001</v>
       </c>
@@ -4101,7 +4141,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A86" s="1">
         <v>345001</v>
       </c>
@@ -4136,7 +4176,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A87" s="1">
         <v>347001</v>
       </c>
@@ -4171,7 +4211,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A88" s="1">
         <v>348001</v>
       </c>
@@ -4206,7 +4246,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A89" s="1">
         <v>351001</v>
       </c>
@@ -4241,7 +4281,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A90" s="1">
         <v>352001</v>
       </c>
@@ -4276,7 +4316,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="91" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A91" s="1">
         <v>391001</v>
       </c>
@@ -4311,7 +4351,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="92" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A92" s="1">
         <v>392001</v>
       </c>
@@ -4346,7 +4386,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="93" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A93" s="1">
         <v>394001</v>
       </c>
@@ -4381,7 +4421,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="94" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A94" s="1">
         <v>395001</v>
       </c>
@@ -4416,7 +4456,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="95" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A95" s="1">
         <v>397001</v>
       </c>
@@ -4451,7 +4491,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="96" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A96" s="1">
         <v>411001</v>
       </c>
@@ -4486,7 +4526,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="97" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A97" s="1">
         <v>412001</v>
       </c>
@@ -4518,7 +4558,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="98" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A98" s="1">
         <v>413001</v>
       </c>
@@ -4550,7 +4590,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="99" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A99" s="1">
         <v>414001</v>
       </c>
@@ -4585,7 +4625,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="100" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A100" s="1">
         <v>415001</v>
       </c>
@@ -4617,7 +4657,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="101" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A101" s="1">
         <v>421001</v>
       </c>
@@ -4649,7 +4689,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="102" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A102" s="1">
         <v>422001</v>
       </c>
@@ -4681,7 +4721,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="103" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A103" s="1">
         <v>431001</v>
       </c>
@@ -4745,7 +4785,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="105" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A105" s="1">
         <v>433001</v>
       </c>
@@ -4777,7 +4817,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="106" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A106" s="1">
         <v>434001</v>
       </c>
@@ -4809,7 +4849,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="107" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A107" s="1">
         <v>441001</v>
       </c>
@@ -4841,7 +4881,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="108" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A108" s="1">
         <v>444001</v>
       </c>
@@ -4873,7 +4913,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="109" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A109" s="1">
         <v>445001</v>
       </c>
@@ -4905,7 +4945,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="110" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A110" s="1">
         <v>446001</v>
       </c>
@@ -4937,7 +4977,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="111" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A111" s="1">
         <v>461001</v>
       </c>
@@ -4969,7 +5009,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="112" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A112" s="1">
         <v>462001</v>
       </c>
@@ -5001,7 +5041,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="113" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A113" s="1">
         <v>463001</v>
       </c>
@@ -5033,7 +5073,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="114" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A114" s="1">
         <v>467001</v>
       </c>
@@ -5065,7 +5105,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="115" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A115" s="1">
         <v>425001</v>
       </c>
@@ -5101,7 +5141,7 @@
       </c>
       <c r="L115" s="1"/>
     </row>
-    <row r="116" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A116" s="1">
         <v>111001</v>
       </c>
@@ -5136,7 +5176,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="117" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A117" s="1">
         <v>101001</v>
       </c>
@@ -5168,6 +5208,216 @@
         <v>15</v>
       </c>
       <c r="K117" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="118" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A118" s="1">
+        <v>100009</v>
+      </c>
+      <c r="B118" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="C118" s="1">
+        <v>0</v>
+      </c>
+      <c r="D118" t="b">
+        <v>0</v>
+      </c>
+      <c r="E118" s="1">
+        <v>4</v>
+      </c>
+      <c r="F118" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="G118" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="H118" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="I118" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="J118" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="K118" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="119" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A119" s="1">
+        <v>100010</v>
+      </c>
+      <c r="B119" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="C119" s="1">
+        <v>0</v>
+      </c>
+      <c r="D119" t="b">
+        <v>0</v>
+      </c>
+      <c r="E119" s="1">
+        <v>4</v>
+      </c>
+      <c r="F119" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="G119" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="H119" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="I119" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="J119" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="K119" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="120" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A120" s="1">
+        <v>100011</v>
+      </c>
+      <c r="B120" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="C120" s="1">
+        <v>0</v>
+      </c>
+      <c r="D120" t="b">
+        <v>0</v>
+      </c>
+      <c r="E120" s="1">
+        <v>4</v>
+      </c>
+      <c r="F120" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="G120" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="H120" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="I120" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="J120" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="K120" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="121" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A121" s="1">
+        <v>100012</v>
+      </c>
+      <c r="B121" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="C121" s="1">
+        <v>0</v>
+      </c>
+      <c r="D121" t="b">
+        <v>0</v>
+      </c>
+      <c r="E121" s="1">
+        <v>4</v>
+      </c>
+      <c r="F121" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="G121" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="H121" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="I121" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="J121" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="K121" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="122" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A122" s="1">
+        <v>100013</v>
+      </c>
+      <c r="B122" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="C122" s="1">
+        <v>0</v>
+      </c>
+      <c r="D122" t="b">
+        <v>0</v>
+      </c>
+      <c r="E122" s="1">
+        <v>4</v>
+      </c>
+      <c r="F122" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="G122" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="H122" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="I122" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="J122" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="K122" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="123" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A123" s="1">
+        <v>100014</v>
+      </c>
+      <c r="B123" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="C123" s="1">
+        <v>0</v>
+      </c>
+      <c r="D123" t="b">
+        <v>0</v>
+      </c>
+      <c r="E123" s="1">
+        <v>4</v>
+      </c>
+      <c r="F123" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="G123" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="H123" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="I123" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="J123" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="K123" s="1" t="s">
         <v>16</v>
       </c>
     </row>

</xml_diff>